<commit_message>
LGHUB 2024/10/12 更新 1
签发：Ling Gao
反馈更新详见：Documents/Update_Feedback.md
平台更新详见：Documents/Update_Platform.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F89EC31-0C19-4059-9CA5-ABAEBE3F4B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A5C424-C1DC-4DF0-A475-969441ADEA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -1758,10 +1758,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -4188,13 +4188,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>144942</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>167443</xdr:rowOff>
+      <xdr:rowOff>171797</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>140819</xdr:rowOff>
+      <xdr:rowOff>145173</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4775,39 +4775,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="D59" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>45572</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>45565</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45537</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45530</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45523</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45516</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45509</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45502</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45495</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45488</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45481</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45474</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45467</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45460</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45453</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45446</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45439</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45432</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45425</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45418</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45411</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45404</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45397</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45390</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45383</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45376</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45369</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45362</v>
       </c>
@@ -5202,7 +5202,7 @@
       </c>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45355</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45348</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45341</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45334</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45327</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45320</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45313</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45306</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -5282,7 +5282,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -5298,7 +5298,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -5314,7 +5314,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -5330,7 +5330,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -5346,7 +5346,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -5362,7 +5362,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -5378,7 +5378,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -5394,7 +5394,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -5410,7 +5410,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -5426,7 +5426,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -5442,7 +5442,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -5458,7 +5458,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -5474,7 +5474,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -5490,7 +5490,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -5506,7 +5506,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -5522,7 +5522,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -5538,7 +5538,7 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
     </row>
-    <row r="75" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -5554,7 +5554,7 @@
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
     </row>
-    <row r="76" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -5570,7 +5570,7 @@
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
     </row>
-    <row r="77" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -5586,7 +5586,7 @@
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
     </row>
-    <row r="78" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -5602,7 +5602,7 @@
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
     </row>
-    <row r="79" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -5618,7 +5618,7 @@
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
     </row>
-    <row r="80" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -5634,7 +5634,7 @@
       <c r="P80" s="2"/>
       <c r="Q80" s="2"/>
     </row>
-    <row r="81" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -5650,7 +5650,7 @@
       <c r="P81" s="2"/>
       <c r="Q81" s="2"/>
     </row>
-    <row r="82" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -5666,7 +5666,7 @@
       <c r="P82" s="2"/>
       <c r="Q82" s="2"/>
     </row>
-    <row r="83" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2024/10/19 更新 1
签发：Ling Gao
反馈更新详见：Documents/Update_Feedback.md
平台更新详见：Documents/Update_Platform.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A5C424-C1DC-4DF0-A475-969441ADEA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AA105F-DB14-41FC-B653-30BC47132957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,54 +917,54 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$24</c:f>
+              <c:f>Sheet1!$C$18:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>45579</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45572</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45565</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45537</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45530</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45523</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45516</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$24</c:f>
+              <c:f>Sheet1!$D$18:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>223</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>218</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>217</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>212</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1068,54 +1068,54 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$24</c:f>
+              <c:f>Sheet1!$C$18:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>45579</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45572</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45565</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45537</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45530</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45523</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45516</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$24</c:f>
+              <c:f>Sheet1!$G$18:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>216</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>207</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>190</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1251,7 +1251,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="240"/>
-          <c:min val="180"/>
+          <c:min val="190"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1758,13 +1758,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4188,13 +4188,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>144942</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>171797</xdr:rowOff>
+      <xdr:rowOff>168687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>145173</xdr:rowOff>
+      <xdr:rowOff>142063</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4775,31 +4775,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D59" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D57" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4807,15 +4807,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="1">
+        <v>45579</v>
+      </c>
+      <c r="D18">
+        <v>231</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45579</v>
+      </c>
+      <c r="G18">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
         <v>45572</v>
       </c>
@@ -4829,7 +4843,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
         <v>45565</v>
       </c>
@@ -4843,7 +4857,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
         <v>45537</v>
       </c>
@@ -4857,7 +4871,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
         <v>45530</v>
       </c>
@@ -4871,7 +4885,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
         <v>45523</v>
       </c>
@@ -4885,7 +4899,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
         <v>45516</v>
       </c>
@@ -4899,7 +4913,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
         <v>45509</v>
       </c>
@@ -4913,7 +4927,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
         <v>45502</v>
       </c>
@@ -4927,7 +4941,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
         <v>45495</v>
       </c>
@@ -4941,7 +4955,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
         <v>45488</v>
       </c>
@@ -4955,7 +4969,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
         <v>45481</v>
       </c>
@@ -4969,7 +4983,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
         <v>45474</v>
       </c>
@@ -4983,7 +4997,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
         <v>45467</v>
       </c>
@@ -4997,7 +5011,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
         <v>45460</v>
       </c>
@@ -5011,7 +5025,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>45453</v>
       </c>
@@ -5025,7 +5039,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
         <v>45446</v>
       </c>
@@ -5039,7 +5053,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
         <v>45439</v>
       </c>
@@ -5053,7 +5067,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
         <v>45432</v>
       </c>
@@ -5067,7 +5081,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
         <v>45425</v>
       </c>
@@ -5081,7 +5095,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
         <v>45418</v>
       </c>
@@ -5095,7 +5109,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
         <v>45411</v>
       </c>
@@ -5109,7 +5123,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
         <v>45404</v>
       </c>
@@ -5123,7 +5137,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
         <v>45397</v>
       </c>
@@ -5137,7 +5151,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
         <v>45390</v>
       </c>
@@ -5151,7 +5165,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
         <v>45383</v>
       </c>
@@ -5165,7 +5179,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
         <v>45376</v>
       </c>
@@ -5179,7 +5193,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
         <v>45369</v>
       </c>
@@ -5193,7 +5207,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
         <v>45362</v>
       </c>
@@ -5202,7 +5216,7 @@
       </c>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
         <v>45355</v>
       </c>
@@ -5210,7 +5224,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
         <v>45348</v>
       </c>
@@ -5218,7 +5232,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
         <v>45341</v>
       </c>
@@ -5226,7 +5240,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
         <v>45334</v>
       </c>
@@ -5234,7 +5248,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
         <v>45327</v>
       </c>
@@ -5242,7 +5256,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
         <v>45320</v>
       </c>
@@ -5250,7 +5264,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
         <v>45313</v>
       </c>
@@ -5258,7 +5272,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
         <v>45306</v>
       </c>
@@ -5266,7 +5280,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -5282,7 +5296,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -5298,7 +5312,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -5314,7 +5328,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -5330,7 +5344,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -5346,7 +5360,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -5362,7 +5376,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -5378,7 +5392,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -5394,7 +5408,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -5410,7 +5424,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -5426,7 +5440,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -5442,7 +5456,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -5458,7 +5472,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -5474,7 +5488,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -5490,7 +5504,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -5506,7 +5520,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -5522,7 +5536,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -5538,7 +5552,7 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
     </row>
-    <row r="75" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -5554,7 +5568,7 @@
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
     </row>
-    <row r="76" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -5570,7 +5584,7 @@
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
     </row>
-    <row r="77" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -5586,7 +5600,7 @@
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
     </row>
-    <row r="78" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -5602,7 +5616,7 @@
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
     </row>
-    <row r="79" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -5618,7 +5632,7 @@
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
     </row>
-    <row r="80" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -5634,7 +5648,7 @@
       <c r="P80" s="2"/>
       <c r="Q80" s="2"/>
     </row>
-    <row r="81" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -5650,7 +5664,7 @@
       <c r="P81" s="2"/>
       <c r="Q81" s="2"/>
     </row>
-    <row r="82" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -5666,7 +5680,7 @@
       <c r="P82" s="2"/>
       <c r="Q82" s="2"/>
     </row>
-    <row r="83" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2024/11/9 更新 1
签发：Ling Gao
反馈更新详见：Documents/Update_Feedback.md
平台更新详见：Documents/Update_Platform.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28217"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B325E6-A22E-449B-B241-442B5C4B2DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093304B0-6A2E-4EF5-8606-49BF39FEEDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,54 +917,54 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$23</c:f>
+              <c:f>Sheet1!$C$17:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>45607</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45579</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45572</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45565</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45537</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45530</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$23</c:f>
+              <c:f>Sheet1!$D$17:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>232</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>231</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>223</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1068,51 +1068,51 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$23</c:f>
+              <c:f>Sheet1!$C$17:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>45607</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45579</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45572</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45565</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45537</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45530</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$23</c:f>
+              <c:f>Sheet1!$G$17:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>207</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>207</c:v>
@@ -1758,13 +1758,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4188,13 +4188,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>144942</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>168687</xdr:rowOff>
+      <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>142063</xdr:rowOff>
+      <xdr:rowOff>138399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4775,47 +4775,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D57" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" topLeftCell="C59" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>45607</v>
+      </c>
+      <c r="D17">
+        <v>237</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45607</v>
+      </c>
+      <c r="G17">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>45600</v>
       </c>
@@ -4829,7 +4847,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>45579</v>
       </c>
@@ -4843,7 +4861,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>45572</v>
       </c>
@@ -4857,7 +4875,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45565</v>
       </c>
@@ -4871,7 +4889,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45537</v>
       </c>
@@ -4885,7 +4903,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45530</v>
       </c>
@@ -4899,7 +4917,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45523</v>
       </c>
@@ -4913,7 +4931,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45516</v>
       </c>
@@ -4927,7 +4945,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45509</v>
       </c>
@@ -4941,7 +4959,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45502</v>
       </c>
@@ -4955,7 +4973,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45495</v>
       </c>
@@ -4969,7 +4987,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45488</v>
       </c>
@@ -4983,7 +5001,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45481</v>
       </c>
@@ -4997,7 +5015,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45474</v>
       </c>
@@ -5011,7 +5029,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45467</v>
       </c>
@@ -5025,7 +5043,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45460</v>
       </c>
@@ -5039,7 +5057,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45453</v>
       </c>
@@ -5053,7 +5071,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45446</v>
       </c>
@@ -5067,7 +5085,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45439</v>
       </c>
@@ -5081,7 +5099,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45432</v>
       </c>
@@ -5095,7 +5113,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45425</v>
       </c>
@@ -5109,7 +5127,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45418</v>
       </c>
@@ -5123,7 +5141,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45411</v>
       </c>
@@ -5137,7 +5155,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45404</v>
       </c>
@@ -5151,7 +5169,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45397</v>
       </c>
@@ -5165,7 +5183,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45390</v>
       </c>
@@ -5179,7 +5197,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45383</v>
       </c>
@@ -5193,7 +5211,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45376</v>
       </c>
@@ -5207,7 +5225,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45369</v>
       </c>
@@ -5221,7 +5239,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45362</v>
       </c>
@@ -5230,7 +5248,7 @@
       </c>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45355</v>
       </c>
@@ -5238,7 +5256,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45348</v>
       </c>
@@ -5246,7 +5264,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45341</v>
       </c>
@@ -5254,7 +5272,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45334</v>
       </c>
@@ -5262,7 +5280,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45327</v>
       </c>
@@ -5270,7 +5288,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45320</v>
       </c>
@@ -5278,7 +5296,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45313</v>
       </c>
@@ -5286,7 +5304,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>45306</v>
       </c>
@@ -5294,7 +5312,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -5310,7 +5328,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -5326,7 +5344,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -5342,7 +5360,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -5358,7 +5376,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -5374,7 +5392,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -5390,7 +5408,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -5406,7 +5424,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -5422,7 +5440,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -5438,7 +5456,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -5454,7 +5472,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -5470,7 +5488,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -5486,7 +5504,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -5502,7 +5520,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -5518,7 +5536,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -5534,7 +5552,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -5550,7 +5568,7 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
     </row>
-    <row r="75" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -5566,7 +5584,7 @@
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
     </row>
-    <row r="76" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -5582,7 +5600,7 @@
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
     </row>
-    <row r="77" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -5598,7 +5616,7 @@
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
     </row>
-    <row r="78" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -5614,7 +5632,7 @@
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
     </row>
-    <row r="79" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -5630,7 +5648,7 @@
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
     </row>
-    <row r="80" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -5646,7 +5664,7 @@
       <c r="P80" s="2"/>
       <c r="Q80" s="2"/>
     </row>
-    <row r="81" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -5662,7 +5680,7 @@
       <c r="P81" s="2"/>
       <c r="Q81" s="2"/>
     </row>
-    <row r="82" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -5678,7 +5696,7 @@
       <c r="P82" s="2"/>
       <c r="Q82" s="2"/>
     </row>
-    <row r="83" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
@@ -5694,7 +5712,7 @@
       <c r="P83" s="2"/>
       <c r="Q83" s="2"/>
     </row>
-    <row r="84" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2024/11/10 更新 2
签发：Ling Gao
反馈更新详见：Documents/Update_Feedback.md
平台更新详见：Documents/Update_Platform.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093304B0-6A2E-4EF5-8606-49BF39FEEDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69750529-C257-4E99-A516-4C1BDA3A59F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4186,7 +4186,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>144942</xdr:colOff>
+      <xdr:colOff>106422</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
@@ -4194,7 +4194,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>138399</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4222,15 +4222,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>271627</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>169007</xdr:rowOff>
+      <xdr:rowOff>169006</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>160920</xdr:colOff>
+      <xdr:colOff>103551</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>143860</xdr:rowOff>
+      <xdr:rowOff>161072</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4775,8 +4775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C59" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C60" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
LGHUB 2024/11/14 更新 1
签发：Ling Gao
- 反馈更新详见：Documents/Update_Feedback.md
- 平台更新详见：Documents/Update_Platform.md
- 更新简报详见：LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69750529-C257-4E99-A516-4C1BDA3A59F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6C8A55-0D72-4580-B887-8DA27FEE3978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,7 +917,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$22</c:f>
+              <c:f>Sheet1!$C$19:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="6"/>
@@ -944,12 +944,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$22</c:f>
+              <c:f>Sheet1!$D$19:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>237</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>232</c:v>
@@ -1068,7 +1068,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$22</c:f>
+              <c:f>Sheet1!$C$19:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1095,12 +1095,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$22</c:f>
+              <c:f>Sheet1!$G$19:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>228</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>227</c:v>
@@ -1758,13 +1758,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4187,13 +4187,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4222,15 +4222,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>169006</xdr:rowOff>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>103551</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>161072</xdr:rowOff>
+      <xdr:colOff>124495</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4773,578 +4773,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q84"/>
+  <dimension ref="B2:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C60" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView tabSelected="1" topLeftCell="E58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19" s="1">
         <v>45607</v>
       </c>
-      <c r="D17">
-        <v>237</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="D19">
+        <v>239</v>
+      </c>
+      <c r="F19" s="1">
         <v>45607</v>
       </c>
-      <c r="G17">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="1">
+      <c r="G19">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C20" s="1">
         <v>45600</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>232</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F20" s="1">
         <v>45600</v>
       </c>
-      <c r="G18">
+      <c r="G20">
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C21" s="1">
         <v>45579</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>231</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F21" s="1">
         <v>45579</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="1">
         <v>45572</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <v>227</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F22" s="1">
         <v>45572</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="1">
         <v>45565</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>223</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F23" s="1">
         <v>45565</v>
       </c>
-      <c r="G21">
+      <c r="G23">
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="1">
         <v>45537</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>218</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F24" s="1">
         <v>45537</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="1">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="1">
         <v>45530</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>217</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F25" s="1">
         <v>45530</v>
       </c>
-      <c r="G23">
+      <c r="G25">
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="1">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="1">
         <v>45523</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <v>216</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F26" s="1">
         <v>45523</v>
       </c>
-      <c r="G24">
+      <c r="G26">
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="1">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C27" s="1">
         <v>45516</v>
       </c>
-      <c r="D25">
+      <c r="D27">
         <v>212</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F27" s="1">
         <v>45516</v>
       </c>
-      <c r="G25">
+      <c r="G27">
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="1">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="1">
         <v>45509</v>
       </c>
-      <c r="D26">
+      <c r="D28">
         <v>210</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F28" s="1">
         <v>45509</v>
       </c>
-      <c r="G26">
+      <c r="G28">
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="1">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="1">
         <v>45502</v>
       </c>
-      <c r="D27">
+      <c r="D29">
         <v>210</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F29" s="1">
         <v>45502</v>
       </c>
-      <c r="G27">
+      <c r="G29">
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="1">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="1">
         <v>45495</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>201</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F30" s="1">
         <v>45495</v>
       </c>
-      <c r="G28">
+      <c r="G30">
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="1">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="1">
         <v>45488</v>
       </c>
-      <c r="D29">
+      <c r="D31">
         <v>199</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F31" s="1">
         <v>45488</v>
       </c>
-      <c r="G29">
+      <c r="G31">
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="1">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C32" s="1">
         <v>45481</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <v>188</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F32" s="1">
         <v>45481</v>
       </c>
-      <c r="G30">
+      <c r="G32">
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="1">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C33" s="1">
         <v>45474</v>
       </c>
-      <c r="D31">
+      <c r="D33">
         <v>187</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F33" s="1">
         <v>45474</v>
       </c>
-      <c r="G31">
+      <c r="G33">
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="1">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C34" s="1">
         <v>45467</v>
       </c>
-      <c r="D32">
+      <c r="D34">
         <v>187</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F34" s="1">
         <v>45467</v>
       </c>
-      <c r="G32">
+      <c r="G34">
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="1">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C35" s="1">
         <v>45460</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <v>185</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F35" s="1">
         <v>45460</v>
       </c>
-      <c r="G33">
+      <c r="G35">
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="1">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C36" s="1">
         <v>45453</v>
       </c>
-      <c r="D34">
+      <c r="D36">
         <v>180</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F36" s="1">
         <v>45453</v>
       </c>
-      <c r="G34">
+      <c r="G36">
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="1">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C37" s="1">
         <v>45446</v>
       </c>
-      <c r="D35">
+      <c r="D37">
         <v>177</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F37" s="1">
         <v>45446</v>
       </c>
-      <c r="G35">
+      <c r="G37">
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="1">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C38" s="1">
         <v>45439</v>
       </c>
-      <c r="D36">
+      <c r="D38">
         <v>174</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F38" s="1">
         <v>45439</v>
       </c>
-      <c r="G36">
+      <c r="G38">
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="1">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C39" s="1">
         <v>45432</v>
       </c>
-      <c r="D37">
+      <c r="D39">
         <v>173</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F39" s="1">
         <v>45432</v>
       </c>
-      <c r="G37">
+      <c r="G39">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="1">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C40" s="1">
         <v>45425</v>
       </c>
-      <c r="D38">
+      <c r="D40">
         <v>170</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F40" s="1">
         <v>45425</v>
       </c>
-      <c r="G38">
+      <c r="G40">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="1">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C41" s="1">
         <v>45418</v>
       </c>
-      <c r="D39">
+      <c r="D41">
         <v>170</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F41" s="1">
         <v>45418</v>
-      </c>
-      <c r="G39">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="1">
-        <v>45411</v>
-      </c>
-      <c r="D40">
-        <v>166</v>
-      </c>
-      <c r="F40" s="1">
-        <v>45411</v>
-      </c>
-      <c r="G40">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="1">
-        <v>45404</v>
-      </c>
-      <c r="D41">
-        <v>166</v>
-      </c>
-      <c r="F41" s="1">
-        <v>45404</v>
       </c>
       <c r="G41">
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
+        <v>45411</v>
+      </c>
+      <c r="D42">
+        <v>166</v>
+      </c>
+      <c r="F42" s="1">
+        <v>45411</v>
+      </c>
+      <c r="G42">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C43" s="1">
+        <v>45404</v>
+      </c>
+      <c r="D43">
+        <v>166</v>
+      </c>
+      <c r="F43" s="1">
+        <v>45404</v>
+      </c>
+      <c r="G43">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C44" s="1">
         <v>45397</v>
       </c>
-      <c r="D42">
+      <c r="D44">
         <v>157</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F44" s="1">
         <v>45397</v>
       </c>
-      <c r="G42">
+      <c r="G44">
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="1">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C45" s="1">
         <v>45390</v>
       </c>
-      <c r="D43">
+      <c r="D45">
         <v>146</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F45" s="1">
         <v>45390</v>
       </c>
-      <c r="G43">
+      <c r="G45">
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="1">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C46" s="1">
         <v>45383</v>
       </c>
-      <c r="D44">
+      <c r="D46">
         <v>138</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F46" s="1">
         <v>45383</v>
       </c>
-      <c r="G44">
+      <c r="G46">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="1">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C47" s="1">
         <v>45376</v>
       </c>
-      <c r="D45">
+      <c r="D47">
         <v>129</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F47" s="1">
         <v>45376</v>
       </c>
-      <c r="G45">
+      <c r="G47">
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="1">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C48" s="1">
         <v>45369</v>
       </c>
-      <c r="D46">
+      <c r="D48">
         <v>123</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F48" s="1">
         <v>45369</v>
       </c>
-      <c r="G46">
+      <c r="G48">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="1">
+    <row r="49" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C49" s="1">
         <v>45362</v>
       </c>
-      <c r="D47">
+      <c r="D49">
         <v>113</v>
       </c>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="1">
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C50" s="1">
         <v>45355</v>
       </c>
-      <c r="D48">
+      <c r="D50">
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C49" s="1">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C51" s="1">
         <v>45348</v>
       </c>
-      <c r="D49">
+      <c r="D51">
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C50" s="1">
+    <row r="52" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C52" s="1">
         <v>45341</v>
       </c>
-      <c r="D50">
+      <c r="D52">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C51" s="1">
+    <row r="53" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C53" s="1">
         <v>45334</v>
       </c>
-      <c r="D51">
+      <c r="D53">
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C52" s="1">
+    <row r="54" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C54" s="1">
         <v>45327</v>
       </c>
-      <c r="D52">
+      <c r="D54">
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C53" s="1">
+    <row r="55" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C55" s="1">
         <v>45320</v>
       </c>
-      <c r="D53">
+      <c r="D55">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C54" s="1">
+    <row r="56" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C56" s="1">
         <v>45313</v>
       </c>
-      <c r="D54">
+      <c r="D56">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C55" s="1">
+    <row r="57" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C57" s="1">
         <v>45306</v>
       </c>
-      <c r="D55">
+      <c r="D57">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-    </row>
-    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-    </row>
-    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -5360,7 +5328,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -5376,7 +5344,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -5392,7 +5360,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -5408,7 +5376,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -5424,7 +5392,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -5440,7 +5408,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -5456,7 +5424,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -5472,7 +5440,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -5488,7 +5456,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -5504,7 +5472,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -5520,7 +5488,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -5536,7 +5504,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -5552,7 +5520,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -5568,7 +5536,7 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
     </row>
-    <row r="75" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -5584,7 +5552,7 @@
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
     </row>
-    <row r="76" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -5600,7 +5568,7 @@
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
     </row>
-    <row r="77" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -5616,7 +5584,7 @@
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
     </row>
-    <row r="78" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -5632,7 +5600,7 @@
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
     </row>
-    <row r="79" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -5648,7 +5616,7 @@
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
     </row>
-    <row r="80" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -5664,7 +5632,7 @@
       <c r="P80" s="2"/>
       <c r="Q80" s="2"/>
     </row>
-    <row r="81" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -5680,7 +5648,7 @@
       <c r="P81" s="2"/>
       <c r="Q81" s="2"/>
     </row>
-    <row r="82" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -5696,7 +5664,7 @@
       <c r="P82" s="2"/>
       <c r="Q82" s="2"/>
     </row>
-    <row r="83" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
@@ -5712,7 +5680,7 @@
       <c r="P83" s="2"/>
       <c r="Q83" s="2"/>
     </row>
-    <row r="84" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
@@ -5728,9 +5696,41 @@
       <c r="P84" s="2"/>
       <c r="Q84" s="2"/>
     </row>
+    <row r="85" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="2"/>
+    </row>
+    <row r="86" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" s="2"/>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D59:Q84"/>
+    <mergeCell ref="D61:Q86"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2024/11/22 更新 1
签发：Ling Gao
- 反馈更新详见：Documents/Update_Feedback.md
- 平台更新详见：Documents/Update_Platform.md
- 更新简报详见：LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6C8A55-0D72-4580-B887-8DA27FEE3978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C3DB27-79DE-4ED7-A62F-05758E933AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,54 +917,54 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$24</c:f>
+              <c:f>Sheet1!$C$18:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>45614</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45579</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45572</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45565</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$24</c:f>
+              <c:f>Sheet1!$D$18:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>239</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>232</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>231</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>223</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1068,54 +1068,54 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$24</c:f>
+              <c:f>Sheet1!$C$18:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>45614</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45579</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45572</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45565</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$24</c:f>
+              <c:f>Sheet1!$G$18:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>207</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1250,8 +1250,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="240"/>
-          <c:min val="190"/>
+          <c:max val="250"/>
+          <c:min val="210"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1357,7 +1357,7 @@
         </c:txPr>
         <c:crossAx val="1374558447"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1758,13 +1758,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4775,8 +4775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="D51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4800,7 +4800,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4816,7 +4816,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="1">
+        <v>45614</v>
+      </c>
+      <c r="D18">
+        <v>241</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45614</v>
+      </c>
+      <c r="G18">
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2024/11/25 更新 1
签发：Ling Gao
- 反馈更新详见：Documents/Update_Feedback.md
- 平台更新详见：Documents/Update_Platform.md
- 更新简报详见：LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C3DB27-79DE-4ED7-A62F-05758E933AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3F8784-151A-47C9-9F1D-25D6C041FFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
@@ -917,26 +917,29 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$23</c:f>
+              <c:f>Sheet1!$C$17:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>45621</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45579</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45572</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45565</c:v>
                 </c:pt>
               </c:numCache>
@@ -944,26 +947,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$23</c:f>
+              <c:f>Sheet1!$D$17:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>241</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>239</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>232</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>231</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>223</c:v>
                 </c:pt>
               </c:numCache>
@@ -1068,26 +1074,29 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$23</c:f>
+              <c:f>Sheet1!$C$17:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>45621</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45579</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45572</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45565</c:v>
                 </c:pt>
               </c:numCache>
@@ -1095,26 +1104,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$23</c:f>
+              <c:f>Sheet1!$G$17:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>222</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>216</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>216</c:v>
                 </c:pt>
               </c:numCache>
@@ -1758,10 +1770,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
@@ -4775,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="D59" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4800,7 +4812,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4808,7 +4820,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4817,6 +4829,20 @@
       </c>
       <c r="C7">
         <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <v>45621</v>
+      </c>
+      <c r="D17">
+        <v>247</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45621</v>
+      </c>
+      <c r="G17">
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2024/11/25 更新 3 (完)
签发：Ling Gao
- 反馈更新详见：Documents/Update_Feedback.md
- 平台更新详见：Documents/Update_Platform.md
- 更新简报详见：LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3F8784-151A-47C9-9F1D-25D6C041FFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4956303F-8AC5-429E-ACCD-2FE38DC5501C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1394,7 +1394,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1402,7 +1402,7 @@
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
@@ -4788,7 +4788,7 @@
   <dimension ref="B2:Q86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D59" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
LGHUB 2024/11/27 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4956303F-8AC5-429E-ACCD-2FE38DC5501C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042AEDD2-2147-4A8D-B2EE-FCC553CD78FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
@@ -1770,10 +1770,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
@@ -4788,7 +4788,7 @@
   <dimension ref="B2:Q86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D59" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4812,7 +4812,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4820,7 +4820,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2024/12/5 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042AEDD2-2147-4A8D-B2EE-FCC553CD78FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4346D116-438D-440C-9383-A01C80AD02BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,60 +917,60 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$23</c:f>
+              <c:f>Sheet1!$C$16:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>45628</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45579</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45572</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$23</c:f>
+              <c:f>Sheet1!$D$16:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>247</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>241</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>239</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>232</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>231</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1074,57 +1074,57 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$23</c:f>
+              <c:f>Sheet1!$C$16:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>45628</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45579</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45572</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$23</c:f>
+              <c:f>Sheet1!$G$16:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>234</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>216</c:v>
@@ -1262,8 +1262,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="250"/>
-          <c:min val="210"/>
+          <c:max val="255"/>
+          <c:min val="215"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1770,13 +1770,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4787,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D59" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4797,38 +4797,52 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>19</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>45628</v>
+      </c>
+      <c r="D16">
+        <v>251</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45628</v>
+      </c>
+      <c r="G16">
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2024/12/12 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4346D116-438D-440C-9383-A01C80AD02BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3ACE7A-93B7-4630-AD77-EAA801257CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,37 +917,37 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$22</c:f>
+              <c:f>Sheet1!$C$18:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>45635</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45579</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$22</c:f>
+              <c:f>Sheet1!$D$18:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -955,22 +955,22 @@
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>247</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>241</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>239</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>232</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>231</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1074,60 +1074,60 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$22</c:f>
+              <c:f>Sheet1!$C$18:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>45635</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45579</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$22</c:f>
+              <c:f>Sheet1!$G$18:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>239</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>234</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1770,13 +1770,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4199,13 +4199,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4235,13 +4235,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4785,10 +4785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q86"/>
+  <dimension ref="B2:Q89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4797,622 +4797,588 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
-        <v>45628</v>
-      </c>
-      <c r="D16">
-        <v>251</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45628</v>
-      </c>
-      <c r="G16">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>45621</v>
-      </c>
-      <c r="D17">
-        <v>247</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45621</v>
-      </c>
-      <c r="G17">
-        <v>234</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C18" s="1">
-        <v>45614</v>
+        <v>45635</v>
       </c>
       <c r="D18">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="F18" s="1">
-        <v>45614</v>
+        <v>45635</v>
       </c>
       <c r="G18">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
-        <v>45607</v>
+        <v>45628</v>
       </c>
       <c r="D19">
+        <v>251</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45628</v>
+      </c>
+      <c r="G19">
         <v>239</v>
-      </c>
-      <c r="F19" s="1">
-        <v>45607</v>
-      </c>
-      <c r="G19">
-        <v>230</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
-        <v>45600</v>
+        <v>45621</v>
       </c>
       <c r="D20">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F20" s="1">
-        <v>45600</v>
+        <v>45621</v>
       </c>
       <c r="G20">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
-        <v>45579</v>
+        <v>45614</v>
       </c>
       <c r="D21">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="F21" s="1">
-        <v>45579</v>
+        <v>45614</v>
       </c>
       <c r="G21">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
-        <v>45572</v>
+        <v>45607</v>
       </c>
       <c r="D22">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="F22" s="1">
-        <v>45572</v>
+        <v>45607</v>
       </c>
       <c r="G22">
-        <v>216</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
-        <v>45565</v>
+        <v>45600</v>
       </c>
       <c r="D23">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="F23" s="1">
-        <v>45565</v>
+        <v>45600</v>
       </c>
       <c r="G23">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
-        <v>45537</v>
+        <v>45579</v>
       </c>
       <c r="D24">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="F24" s="1">
-        <v>45537</v>
+        <v>45579</v>
       </c>
       <c r="G24">
-        <v>207</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
-        <v>45530</v>
+        <v>45572</v>
       </c>
       <c r="D25">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="F25" s="1">
-        <v>45530</v>
+        <v>45572</v>
       </c>
       <c r="G25">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>45523</v>
+        <v>45565</v>
       </c>
       <c r="D26">
+        <v>223</v>
+      </c>
+      <c r="F26" s="1">
+        <v>45565</v>
+      </c>
+      <c r="G26">
         <v>216</v>
-      </c>
-      <c r="F26" s="1">
-        <v>45523</v>
-      </c>
-      <c r="G26">
-        <v>200</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>45516</v>
+        <v>45537</v>
       </c>
       <c r="D27">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="F27" s="1">
-        <v>45516</v>
+        <v>45537</v>
       </c>
       <c r="G27">
-        <v>190</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>45509</v>
+        <v>45530</v>
       </c>
       <c r="D28">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="F28" s="1">
-        <v>45509</v>
+        <v>45530</v>
       </c>
       <c r="G28">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>45502</v>
+        <v>45523</v>
       </c>
       <c r="D29">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="F29" s="1">
-        <v>45502</v>
+        <v>45523</v>
       </c>
       <c r="G29">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>45495</v>
+        <v>45516</v>
       </c>
       <c r="D30">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="F30" s="1">
-        <v>45495</v>
+        <v>45516</v>
       </c>
       <c r="G30">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>45488</v>
+        <v>45509</v>
       </c>
       <c r="D31">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="F31" s="1">
-        <v>45488</v>
+        <v>45509</v>
       </c>
       <c r="G31">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>45481</v>
+        <v>45502</v>
       </c>
       <c r="D32">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="F32" s="1">
-        <v>45481</v>
+        <v>45502</v>
       </c>
       <c r="G32">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>45474</v>
+        <v>45495</v>
       </c>
       <c r="D33">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="F33" s="1">
-        <v>45474</v>
+        <v>45495</v>
       </c>
       <c r="G33">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
-        <v>45467</v>
+        <v>45488</v>
       </c>
       <c r="D34">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="F34" s="1">
-        <v>45467</v>
+        <v>45488</v>
       </c>
       <c r="G34">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
-        <v>45460</v>
+        <v>45481</v>
       </c>
       <c r="D35">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F35" s="1">
-        <v>45460</v>
+        <v>45481</v>
       </c>
       <c r="G35">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>45453</v>
+        <v>45474</v>
       </c>
       <c r="D36">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="F36" s="1">
-        <v>45453</v>
+        <v>45474</v>
       </c>
       <c r="G36">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
-        <v>45446</v>
+        <v>45467</v>
       </c>
       <c r="D37">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="F37" s="1">
-        <v>45446</v>
+        <v>45467</v>
       </c>
       <c r="G37">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
-        <v>45439</v>
+        <v>45460</v>
       </c>
       <c r="D38">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F38" s="1">
-        <v>45439</v>
+        <v>45460</v>
       </c>
       <c r="G38">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
-        <v>45432</v>
+        <v>45453</v>
       </c>
       <c r="D39">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F39" s="1">
-        <v>45432</v>
+        <v>45453</v>
       </c>
       <c r="G39">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
-        <v>45425</v>
+        <v>45446</v>
       </c>
       <c r="D40">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F40" s="1">
-        <v>45425</v>
+        <v>45446</v>
       </c>
       <c r="G40">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <v>45418</v>
+        <v>45439</v>
       </c>
       <c r="D41">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F41" s="1">
-        <v>45418</v>
+        <v>45439</v>
       </c>
       <c r="G41">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
-        <v>45411</v>
+        <v>45432</v>
       </c>
       <c r="D42">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F42" s="1">
-        <v>45411</v>
+        <v>45432</v>
       </c>
       <c r="G42">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
-        <v>45404</v>
+        <v>45425</v>
       </c>
       <c r="D43">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F43" s="1">
-        <v>45404</v>
+        <v>45425</v>
       </c>
       <c r="G43">
-        <v>141</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
-        <v>45397</v>
+        <v>45418</v>
       </c>
       <c r="D44">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="F44" s="1">
-        <v>45397</v>
+        <v>45418</v>
       </c>
       <c r="G44">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
-        <v>45390</v>
+        <v>45411</v>
       </c>
       <c r="D45">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="F45" s="1">
-        <v>45390</v>
+        <v>45411</v>
       </c>
       <c r="G45">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
-        <v>45383</v>
+        <v>45404</v>
       </c>
       <c r="D46">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="F46" s="1">
-        <v>45383</v>
+        <v>45404</v>
       </c>
       <c r="G46">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
-        <v>45376</v>
+        <v>45397</v>
       </c>
       <c r="D47">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="F47" s="1">
-        <v>45376</v>
+        <v>45397</v>
       </c>
       <c r="G47">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
-        <v>45369</v>
+        <v>45390</v>
       </c>
       <c r="D48">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="F48" s="1">
-        <v>45369</v>
+        <v>45390</v>
       </c>
       <c r="G48">
-        <v>97</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
-        <v>45362</v>
+        <v>45383</v>
       </c>
       <c r="D49">
-        <v>113</v>
-      </c>
-      <c r="F49" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="F49" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G49">
+        <v>119</v>
+      </c>
     </row>
     <row r="50" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
-        <v>45355</v>
+        <v>45376</v>
       </c>
       <c r="D50">
-        <v>108</v>
+        <v>129</v>
+      </c>
+      <c r="F50" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G50">
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
-        <v>45348</v>
+        <v>45369</v>
       </c>
       <c r="D51">
-        <v>102</v>
+        <v>123</v>
+      </c>
+      <c r="F51" s="1">
+        <v>45369</v>
+      </c>
+      <c r="G51">
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
-        <v>45341</v>
+        <v>45362</v>
       </c>
       <c r="D52">
-        <v>95</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F52" s="1"/>
     </row>
     <row r="53" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
-        <v>45334</v>
+        <v>45355</v>
       </c>
       <c r="D53">
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
-        <v>45327</v>
+        <v>45348</v>
       </c>
       <c r="D54">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
-        <v>45320</v>
+        <v>45341</v>
       </c>
       <c r="D55">
-        <v>55</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
-        <v>45313</v>
+        <v>45334</v>
       </c>
       <c r="D56">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
+        <v>45327</v>
+      </c>
+      <c r="D57">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C58" s="1">
+        <v>45320</v>
+      </c>
+      <c r="D58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C59" s="1">
+        <v>45313</v>
+      </c>
+      <c r="D59">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C60" s="1">
         <v>45306</v>
       </c>
-      <c r="D57">
+      <c r="D60">
         <v>52</v>
       </c>
-    </row>
-    <row r="61" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
-      <c r="O61" s="2"/>
-      <c r="P61" s="2"/>
-      <c r="Q61" s="2"/>
-    </row>
-    <row r="62" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-    </row>
-    <row r="63" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
     </row>
     <row r="64" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D64" s="2"/>
@@ -5782,9 +5748,57 @@
       <c r="P86" s="2"/>
       <c r="Q86" s="2"/>
     </row>
+    <row r="87" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+    </row>
+    <row r="88" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+      <c r="K88" s="2"/>
+      <c r="L88" s="2"/>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+      <c r="O88" s="2"/>
+      <c r="P88" s="2"/>
+      <c r="Q88" s="2"/>
+    </row>
+    <row r="89" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="2"/>
+      <c r="P89" s="2"/>
+      <c r="Q89" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D61:Q86"/>
+    <mergeCell ref="D64:Q89"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2024/12/20 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3ACE7A-93B7-4630-AD77-EAA801257CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F19459-2390-4677-9D6B-C59628615C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,29 +917,32 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$24</c:f>
+              <c:f>Sheet1!$C$17:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45642</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45579</c:v>
                 </c:pt>
               </c:numCache>
@@ -947,29 +950,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$24</c:f>
+              <c:f>Sheet1!$D$17:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>251</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>247</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>241</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>239</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>232</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>231</c:v>
                 </c:pt>
               </c:numCache>
@@ -1074,29 +1080,32 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$24</c:f>
+              <c:f>Sheet1!$C$17:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45642</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45600</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45579</c:v>
                 </c:pt>
               </c:numCache>
@@ -1104,29 +1113,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$24</c:f>
+              <c:f>Sheet1!$G$17:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>243</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>222</c:v>
                 </c:pt>
               </c:numCache>
@@ -1262,8 +1274,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="255"/>
-          <c:min val="215"/>
+          <c:max val="260"/>
+          <c:min val="220"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1770,13 +1782,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4787,8 +4799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M62" sqref="M62"/>
+    <sheetView tabSelected="1" topLeftCell="D62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4812,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4820,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4828,7 +4840,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>28</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <v>45642</v>
+      </c>
+      <c r="D17">
+        <v>256</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45642</v>
+      </c>
+      <c r="G17">
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/1/5 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F19459-2390-4677-9D6B-C59628615C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0589E02-D85C-4B85-A374-462494683978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,40 +917,40 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$24</c:f>
+              <c:f>Sheet1!$C$16:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45663</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45600</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$24</c:f>
+              <c:f>Sheet1!$D$16:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -958,25 +958,25 @@
                   <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>251</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>247</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>241</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>239</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,66 +1080,66 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$24</c:f>
+              <c:f>Sheet1!$C$16:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45663</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45607</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45600</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$24</c:f>
+              <c:f>Sheet1!$G$16:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>245</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>243</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1517,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>(9</a:t>
+              <a:t>(1</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -1543,7 +1543,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>- 12</a:t>
+              <a:t>- 4</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -1782,13 +1782,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4800,7 +4800,7 @@
   <dimension ref="B2:Q89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4809,38 +4809,52 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>45663</v>
+      </c>
+      <c r="D16">
+        <v>256</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45663</v>
+      </c>
+      <c r="G16">
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/1/10 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0589E02-D85C-4B85-A374-462494683978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72065A18-6F58-45B4-924B-CADFED0DAF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -917,66 +917,66 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$23</c:f>
+              <c:f>Sheet1!$C$15:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45670</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45607</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$23</c:f>
+              <c:f>Sheet1!$D$15:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>256</c:v>
+                  <c:v>263</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>251</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>247</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>241</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,40 +1080,40 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$23</c:f>
+              <c:f>Sheet1!$C$15:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45670</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45614</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45607</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$23</c:f>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1121,25 +1121,25 @@
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>245</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>243</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>230</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>227</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1274,8 +1274,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="260"/>
-          <c:min val="220"/>
+          <c:max val="270"/>
+          <c:min val="225"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1782,10 +1782,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -4799,8 +4799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" topLeftCell="D63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4824,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
@@ -4832,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
@@ -4841,6 +4841,20 @@
       </c>
       <c r="C7">
         <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C15" s="1">
+        <v>45670</v>
+      </c>
+      <c r="D15">
+        <v>263</v>
+      </c>
+      <c r="F15" s="1">
+        <v>45670</v>
+      </c>
+      <c r="G15">
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/1/12 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72065A18-6F58-45B4-924B-CADFED0DAF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E9AD9F-C9DB-49F3-859A-B29D75C05739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,7 +577,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -955,7 +955,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>263</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>256</c:v>
@@ -1785,7 +1785,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -4800,7 +4800,7 @@
   <dimension ref="B2:Q89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4832,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
@@ -4848,7 +4848,7 @@
         <v>45670</v>
       </c>
       <c r="D15">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F15" s="1">
         <v>45670</v>

</xml_diff>

<commit_message>
LGHUB 2025/1/17 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E9AD9F-C9DB-49F3-859A-B29D75C05739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBA3C98-F4B9-4DB3-9ED0-2BC3092509C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,66 +917,66 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$C$22</c:f>
+              <c:f>Sheet1!$C$19:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45677</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45614</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$15:$D$22</c:f>
+              <c:f>Sheet1!$D$19:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>264</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>256</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>251</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>247</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>241</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,66 +1080,66 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$C$22</c:f>
+              <c:f>Sheet1!$C$19:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45677</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45621</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45614</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:f>Sheet1!$G$19:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>245</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>243</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>230</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1275,7 +1275,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="270"/>
-          <c:min val="225"/>
+          <c:min val="230"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1782,13 +1782,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4211,13 +4211,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4247,13 +4247,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4797,10 +4797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q89"/>
+  <dimension ref="B2:Q94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="D67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4809,712 +4809,646 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C15" s="1">
-        <v>45670</v>
-      </c>
-      <c r="D15">
-        <v>264</v>
-      </c>
-      <c r="F15" s="1">
-        <v>45670</v>
-      </c>
-      <c r="G15">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
-        <v>45663</v>
-      </c>
-      <c r="D16">
-        <v>256</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45663</v>
-      </c>
-      <c r="G16">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>45642</v>
-      </c>
-      <c r="D17">
-        <v>256</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45642</v>
-      </c>
-      <c r="G17">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="1">
-        <v>45635</v>
-      </c>
-      <c r="D18">
-        <v>251</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45635</v>
-      </c>
-      <c r="G18">
-        <v>243</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="D19">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="F19" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="G19">
-        <v>239</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="D20">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="F20" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="G20">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="D21">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F21" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="G21">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="D22">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="F22" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="G22">
-        <v>230</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="D23">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F23" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="G23">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="D24">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="F24" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="G24">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="D25">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="F25" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="G25">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="D26">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="F26" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="G26">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="D27">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="F27" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="G27">
-        <v>207</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="D28">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="F28" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="G28">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="D29">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="F29" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="G29">
-        <v>200</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="D30">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="F30" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="G30">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="D31">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="F31" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="G31">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="D32">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F32" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="G32">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="D33">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="F33" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="G33">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="D34">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="F34" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="G34">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="D35">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="F35" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="G35">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="D36">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F36" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="G36">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="D37">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F37" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="G37">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="D38">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F38" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="G38">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="D39">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="F39" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="G39">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="D40">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F40" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="G40">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="D41">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F41" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="G41">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="D42">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F42" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="G42">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="D43">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="F43" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="G43">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="D44">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F44" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="G44">
-        <v>141</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="D45">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F45" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="G45">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="D46">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F46" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="G46">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="D47">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F47" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="G47">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
+        <v>45425</v>
+      </c>
+      <c r="D48">
+        <v>170</v>
+      </c>
+      <c r="F48" s="1">
+        <v>45425</v>
+      </c>
+      <c r="G48">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C49" s="1">
+        <v>45418</v>
+      </c>
+      <c r="D49">
+        <v>170</v>
+      </c>
+      <c r="F49" s="1">
+        <v>45418</v>
+      </c>
+      <c r="G49">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C50" s="1">
+        <v>45411</v>
+      </c>
+      <c r="D50">
+        <v>166</v>
+      </c>
+      <c r="F50" s="1">
+        <v>45411</v>
+      </c>
+      <c r="G50">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C51" s="1">
+        <v>45404</v>
+      </c>
+      <c r="D51">
+        <v>166</v>
+      </c>
+      <c r="F51" s="1">
+        <v>45404</v>
+      </c>
+      <c r="G51">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C52" s="1">
+        <v>45397</v>
+      </c>
+      <c r="D52">
+        <v>157</v>
+      </c>
+      <c r="F52" s="1">
+        <v>45397</v>
+      </c>
+      <c r="G52">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C53" s="1">
         <v>45390</v>
       </c>
-      <c r="D48">
+      <c r="D53">
         <v>146</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F53" s="1">
         <v>45390</v>
       </c>
-      <c r="G48">
+      <c r="G53">
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C49" s="1">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C54" s="1">
         <v>45383</v>
       </c>
-      <c r="D49">
+      <c r="D54">
         <v>138</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F54" s="1">
         <v>45383</v>
       </c>
-      <c r="G49">
+      <c r="G54">
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C50" s="1">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C55" s="1">
         <v>45376</v>
       </c>
-      <c r="D50">
+      <c r="D55">
         <v>129</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F55" s="1">
         <v>45376</v>
       </c>
-      <c r="G50">
+      <c r="G55">
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C51" s="1">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C56" s="1">
         <v>45369</v>
       </c>
-      <c r="D51">
+      <c r="D56">
         <v>123</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F56" s="1">
         <v>45369</v>
       </c>
-      <c r="G51">
+      <c r="G56">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C52" s="1">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C57" s="1">
         <v>45362</v>
       </c>
-      <c r="D52">
+      <c r="D57">
         <v>113</v>
       </c>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C53" s="1">
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C58" s="1">
         <v>45355</v>
       </c>
-      <c r="D53">
+      <c r="D58">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C54" s="1">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C59" s="1">
         <v>45348</v>
       </c>
-      <c r="D54">
+      <c r="D59">
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C55" s="1">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C60" s="1">
         <v>45341</v>
       </c>
-      <c r="D55">
+      <c r="D60">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C56" s="1">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C61" s="1">
         <v>45334</v>
       </c>
-      <c r="D56">
+      <c r="D61">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C57" s="1">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C62" s="1">
         <v>45327</v>
       </c>
-      <c r="D57">
+      <c r="D62">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C58" s="1">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C63" s="1">
         <v>45320</v>
       </c>
-      <c r="D58">
+      <c r="D63">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C59" s="1">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C64" s="1">
         <v>45313</v>
       </c>
-      <c r="D59">
+      <c r="D64">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C60" s="1">
+    <row r="65" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C65" s="1">
         <v>45306</v>
       </c>
-      <c r="D60">
+      <c r="D65">
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
-      <c r="P64" s="2"/>
-      <c r="Q64" s="2"/>
-    </row>
-    <row r="65" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="2"/>
-      <c r="N65" s="2"/>
-      <c r="O65" s="2"/>
-      <c r="P65" s="2"/>
-      <c r="Q65" s="2"/>
-    </row>
-    <row r="66" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
-      <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
-    </row>
-    <row r="67" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-    </row>
-    <row r="68" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
-      <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
-      <c r="P68" s="2"/>
-      <c r="Q68" s="2"/>
-    </row>
-    <row r="69" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -5530,7 +5464,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -5546,7 +5480,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -5562,7 +5496,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -5578,7 +5512,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -5594,7 +5528,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -5610,7 +5544,7 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
     </row>
-    <row r="75" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -5626,7 +5560,7 @@
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
     </row>
-    <row r="76" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -5642,7 +5576,7 @@
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
     </row>
-    <row r="77" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -5658,7 +5592,7 @@
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
     </row>
-    <row r="78" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -5674,7 +5608,7 @@
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
     </row>
-    <row r="79" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -5690,7 +5624,7 @@
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
     </row>
-    <row r="80" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -5850,9 +5784,89 @@
       <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
     </row>
+    <row r="90" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
+      <c r="O90" s="2"/>
+      <c r="P90" s="2"/>
+      <c r="Q90" s="2"/>
+    </row>
+    <row r="91" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="2"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="2"/>
+      <c r="P91" s="2"/>
+      <c r="Q91" s="2"/>
+    </row>
+    <row r="92" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" s="2"/>
+      <c r="Q92" s="2"/>
+    </row>
+    <row r="93" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" s="2"/>
+      <c r="P93" s="2"/>
+      <c r="Q93" s="2"/>
+    </row>
+    <row r="94" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+      <c r="O94" s="2"/>
+      <c r="P94" s="2"/>
+      <c r="Q94" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D64:Q89"/>
+    <mergeCell ref="D69:Q94"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/1/20 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBA3C98-F4B9-4DB3-9ED0-2BC3092509C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555F03E7-7FC6-448E-BD83-55DF40F6A76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -955,7 +955,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>265</c:v>
+                  <c:v>273</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>264</c:v>
@@ -1274,7 +1274,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="270"/>
+          <c:max val="280"/>
           <c:min val="230"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1782,7 +1782,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -4799,8 +4799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+    <sheetView tabSelected="1" topLeftCell="D66" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O68" sqref="O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4824,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4848,7 +4848,7 @@
         <v>45677</v>
       </c>
       <c r="D19">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="F19" s="1">
         <v>45677</v>

</xml_diff>

<commit_message>
LGHUB 2025/1/26 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555F03E7-7FC6-448E-BD83-55DF40F6A76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9463D4E1-A11F-4087-A9CE-CA77C6735645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9</c:v>
@@ -917,66 +917,66 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$26</c:f>
+              <c:f>Sheet1!$C$18:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45684</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45621</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$26</c:f>
+              <c:f>Sheet1!$D$18:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>273</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>251</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>247</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>241</c:v>
+                  <c:v>247</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,40 +1080,40 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$26</c:f>
+              <c:f>Sheet1!$C$18:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45684</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45628</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45621</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$26</c:f>
+              <c:f>Sheet1!$G$18:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1121,22 +1121,22 @@
                   <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>245</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>243</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>234</c:v>
@@ -1782,10 +1782,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9</c:v>
@@ -4799,8 +4799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D66" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O68" sqref="O68"/>
+    <sheetView tabSelected="1" topLeftCell="D69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4824,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4832,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4841,6 +4841,20 @@
       </c>
       <c r="C7">
         <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="1">
+        <v>45684</v>
+      </c>
+      <c r="D18">
+        <v>277</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45684</v>
+      </c>
+      <c r="G18">
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/1/29 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9463D4E1-A11F-4087-A9CE-CA77C6735645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEAA0C6-91DD-46FD-928F-F7DBC85609B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9</c:v>
@@ -955,7 +955,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>277</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>273</c:v>
@@ -1274,7 +1274,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="280"/>
+          <c:max val="290"/>
           <c:min val="230"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1782,10 +1782,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9</c:v>
@@ -4799,8 +4799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="D68" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4824,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4832,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4848,7 +4848,7 @@
         <v>45684</v>
       </c>
       <c r="D18">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F18" s="1">
         <v>45684</v>

</xml_diff>

<commit_message>
LGHUB 2025/1/30 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEAA0C6-91DD-46FD-928F-F7DBC85609B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DC2A1E-B796-4FFE-A289-142B50FD9C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -955,7 +955,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>283</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>273</c:v>
@@ -1118,7 +1118,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>254</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>254</c:v>
@@ -1782,13 +1782,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4800,7 +4800,7 @@
   <dimension ref="B2:Q94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D68" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4824,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4832,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4840,7 +4840,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">
@@ -4848,13 +4848,13 @@
         <v>45684</v>
       </c>
       <c r="D18">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F18" s="1">
         <v>45684</v>
       </c>
       <c r="G18">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/2/1 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DC2A1E-B796-4FFE-A289-142B50FD9C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E51937-259C-447A-BB05-6CB0C74DFD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -917,66 +917,66 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$25</c:f>
+              <c:f>Sheet1!$C$17:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45691</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45628</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$25</c:f>
+              <c:f>Sheet1!$D$17:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>284</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>273</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>251</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>247</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,40 +1080,40 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$25</c:f>
+              <c:f>Sheet1!$C$17:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45691</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45642</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45635</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45628</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$25</c:f>
+              <c:f>Sheet1!$G$17:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1121,25 +1121,25 @@
                   <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>254</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>250</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>245</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>243</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1782,7 +1782,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -4799,8 +4799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D68" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="D67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4824,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4841,6 +4841,20 @@
       </c>
       <c r="C7">
         <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <v>45691</v>
+      </c>
+      <c r="D17">
+        <v>287</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45691</v>
+      </c>
+      <c r="G17">
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/2/6 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E51937-259C-447A-BB05-6CB0C74DFD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC31A29-5B6A-4DE0-B2A4-E0A50B567C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -955,7 +955,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>287</c:v>
+                  <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>284</c:v>
@@ -1118,7 +1118,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>262</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>262</c:v>
@@ -1782,13 +1782,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4800,7 +4800,7 @@
   <dimension ref="B2:Q94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K66" sqref="K66"/>
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4824,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4832,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4840,7 +4840,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">
@@ -4848,13 +4848,13 @@
         <v>45691</v>
       </c>
       <c r="D17">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F17" s="1">
         <v>45691</v>
       </c>
       <c r="G17">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/2/22 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC31A29-5B6A-4DE0-B2A4-E0A50B567C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B1B704-0DE8-49DB-8C1C-9AF742C3900A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22</c:v>
@@ -917,66 +917,66 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$24</c:f>
+              <c:f>Sheet1!$C$15:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45705</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45698</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>45642</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45635</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$24</c:f>
+              <c:f>Sheet1!$D$15:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>289</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>284</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>273</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>264</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>251</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,40 +1080,40 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$24</c:f>
+              <c:f>Sheet1!$C$15:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>45705</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45698</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>45642</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45635</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$24</c:f>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1121,25 +1121,25 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>262</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>254</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>243</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1274,8 +1274,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="290"/>
-          <c:min val="230"/>
+          <c:max val="310"/>
+          <c:min val="240"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1782,10 +1782,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22</c:v>
@@ -4800,7 +4800,7 @@
   <dimension ref="B2:Q94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+      <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4809,38 +4809,66 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
         <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C15" s="1">
+        <v>45705</v>
+      </c>
+      <c r="D15">
+        <v>301</v>
+      </c>
+      <c r="F15" s="1">
+        <v>45705</v>
+      </c>
+      <c r="G15">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>45698</v>
+      </c>
+      <c r="D16">
+        <v>295</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45698</v>
+      </c>
+      <c r="G16">
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/3/1 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B1B704-0DE8-49DB-8C1C-9AF742C3900A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0932098-DE49-468B-9DF3-7D4303DD9CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,32 +917,35 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$C$22</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45712</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45642</c:v>
                 </c:pt>
               </c:numCache>
@@ -950,32 +953,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$15:$D$22</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>301</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>289</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>284</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>273</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>264</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
@@ -1080,32 +1086,35 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$C$22</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45712</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45663</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45642</c:v>
                 </c:pt>
               </c:numCache>
@@ -1113,12 +1122,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>267</c:v>
@@ -1127,18 +1136,21 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>262</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>245</c:v>
                 </c:pt>
               </c:numCache>
@@ -1782,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4211,13 +4223,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4247,13 +4259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4797,10 +4809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q94"/>
+  <dimension ref="B2:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M68" sqref="M68"/>
+    <sheetView tabSelected="1" topLeftCell="D73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4809,780 +4821,714 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C15" s="1">
-        <v>45705</v>
-      </c>
-      <c r="D15">
-        <v>301</v>
-      </c>
-      <c r="F15" s="1">
-        <v>45705</v>
-      </c>
-      <c r="G15">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
-        <v>45698</v>
-      </c>
-      <c r="D16">
-        <v>295</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45698</v>
-      </c>
-      <c r="G16">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>45691</v>
-      </c>
-      <c r="D17">
-        <v>289</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45691</v>
-      </c>
-      <c r="G17">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="1">
-        <v>45684</v>
-      </c>
-      <c r="D18">
-        <v>284</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45684</v>
-      </c>
-      <c r="G18">
-        <v>262</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
-        <v>45677</v>
+        <v>45712</v>
       </c>
       <c r="D19">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="F19" s="1">
-        <v>45677</v>
+        <v>45712</v>
       </c>
       <c r="G19">
-        <v>254</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
-        <v>45670</v>
+        <v>45705</v>
       </c>
       <c r="D20">
-        <v>264</v>
+        <v>301</v>
       </c>
       <c r="F20" s="1">
-        <v>45670</v>
+        <v>45705</v>
       </c>
       <c r="G20">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="D21">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="F21" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="G21">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
-        <v>45642</v>
+        <v>45691</v>
       </c>
       <c r="D22">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="F22" s="1">
-        <v>45642</v>
+        <v>45691</v>
       </c>
       <c r="G22">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
-        <v>45635</v>
+        <v>45684</v>
       </c>
       <c r="D23">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="F23" s="1">
-        <v>45635</v>
+        <v>45684</v>
       </c>
       <c r="G23">
-        <v>243</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="D24">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="F24" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="G24">
-        <v>239</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="D25">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="F25" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="G25">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="D26">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F26" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="G26">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="D27">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="F27" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="G27">
-        <v>230</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="D28">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F28" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="G28">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="D29">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="F29" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="G29">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="D30">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="F30" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="G30">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="D31">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="F31" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="G31">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="D32">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="F32" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="G32">
-        <v>207</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="D33">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="F33" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="G33">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="D34">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="F34" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="G34">
-        <v>200</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="D35">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="F35" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="G35">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="D36">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="F36" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="G36">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="D37">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F37" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="G37">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="D38">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="F38" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="G38">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="D39">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="F39" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="G39">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="D40">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="F40" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="G40">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="D41">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F41" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="G41">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="D42">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F42" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="G42">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="D43">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F43" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="G43">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="D44">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="F44" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="G44">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="D45">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F45" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="G45">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="D46">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F46" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="G46">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="D47">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F47" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="G47">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="D48">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="F48" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="G48">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="D49">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F49" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="G49">
-        <v>141</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="D50">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F50" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="G50">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="D51">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F51" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="G51">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="D52">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F52" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="G52">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
-        <v>45390</v>
+        <v>45425</v>
       </c>
       <c r="D53">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="F53" s="1">
-        <v>45390</v>
+        <v>45425</v>
       </c>
       <c r="G53">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
-        <v>45383</v>
+        <v>45418</v>
       </c>
       <c r="D54">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F54" s="1">
-        <v>45383</v>
+        <v>45418</v>
       </c>
       <c r="G54">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
-        <v>45376</v>
+        <v>45411</v>
       </c>
       <c r="D55">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="F55" s="1">
-        <v>45376</v>
+        <v>45411</v>
       </c>
       <c r="G55">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
-        <v>45369</v>
+        <v>45404</v>
       </c>
       <c r="D56">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="F56" s="1">
-        <v>45369</v>
+        <v>45404</v>
       </c>
       <c r="G56">
-        <v>97</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
-        <v>45362</v>
+        <v>45397</v>
       </c>
       <c r="D57">
-        <v>113</v>
-      </c>
-      <c r="F57" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="F57" s="1">
+        <v>45397</v>
+      </c>
+      <c r="G57">
+        <v>132</v>
+      </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
-        <v>45355</v>
+        <v>45390</v>
       </c>
       <c r="D58">
-        <v>108</v>
+        <v>146</v>
+      </c>
+      <c r="F58" s="1">
+        <v>45390</v>
+      </c>
+      <c r="G58">
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
-        <v>45348</v>
+        <v>45383</v>
       </c>
       <c r="D59">
-        <v>102</v>
+        <v>138</v>
+      </c>
+      <c r="F59" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G59">
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
-        <v>45341</v>
+        <v>45376</v>
       </c>
       <c r="D60">
-        <v>95</v>
+        <v>129</v>
+      </c>
+      <c r="F60" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G60">
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
-        <v>45334</v>
+        <v>45369</v>
       </c>
       <c r="D61">
-        <v>80</v>
+        <v>123</v>
+      </c>
+      <c r="F61" s="1">
+        <v>45369</v>
+      </c>
+      <c r="G61">
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
-        <v>45327</v>
+        <v>45362</v>
       </c>
       <c r="D62">
-        <v>66</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F62" s="1"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
-        <v>45320</v>
+        <v>45355</v>
       </c>
       <c r="D63">
-        <v>55</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
-        <v>45313</v>
+        <v>45348</v>
       </c>
       <c r="D64">
-        <v>53</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
+        <v>45341</v>
+      </c>
+      <c r="D65">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C66" s="1">
+        <v>45334</v>
+      </c>
+      <c r="D66">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C67" s="1">
+        <v>45327</v>
+      </c>
+      <c r="D67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C68" s="1">
+        <v>45320</v>
+      </c>
+      <c r="D68">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C69" s="1">
+        <v>45313</v>
+      </c>
+      <c r="D69">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C70" s="1">
         <v>45306</v>
       </c>
-      <c r="D65">
+      <c r="D70">
         <v>52</v>
       </c>
-    </row>
-    <row r="69" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
-      <c r="O69" s="2"/>
-      <c r="P69" s="2"/>
-      <c r="Q69" s="2"/>
-    </row>
-    <row r="70" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
-      <c r="Q70" s="2"/>
-    </row>
-    <row r="71" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
-      <c r="P71" s="2"/>
-      <c r="Q71" s="2"/>
-    </row>
-    <row r="72" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="K72" s="2"/>
-      <c r="L72" s="2"/>
-      <c r="M72" s="2"/>
-      <c r="N72" s="2"/>
-      <c r="O72" s="2"/>
-      <c r="P72" s="2"/>
-      <c r="Q72" s="2"/>
-    </row>
-    <row r="73" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
-      <c r="O73" s="2"/>
-      <c r="P73" s="2"/>
-      <c r="Q73" s="2"/>
     </row>
     <row r="74" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D74" s="2"/>
@@ -5920,9 +5866,89 @@
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
     </row>
+    <row r="95" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2"/>
+      <c r="N95" s="2"/>
+      <c r="O95" s="2"/>
+      <c r="P95" s="2"/>
+      <c r="Q95" s="2"/>
+    </row>
+    <row r="96" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
+      <c r="N96" s="2"/>
+      <c r="O96" s="2"/>
+      <c r="P96" s="2"/>
+      <c r="Q96" s="2"/>
+    </row>
+    <row r="97" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+      <c r="O97" s="2"/>
+      <c r="P97" s="2"/>
+      <c r="Q97" s="2"/>
+    </row>
+    <row r="98" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
+      <c r="L98" s="2"/>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" s="2"/>
+      <c r="P98" s="2"/>
+      <c r="Q98" s="2"/>
+    </row>
+    <row r="99" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
+      <c r="L99" s="2"/>
+      <c r="M99" s="2"/>
+      <c r="N99" s="2"/>
+      <c r="O99" s="2"/>
+      <c r="P99" s="2"/>
+      <c r="Q99" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D69:Q94"/>
+    <mergeCell ref="D74:Q99"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/3/2 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0932098-DE49-468B-9DF3-7D4303DD9CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09D81B1-30A7-40CF-BDA7-D06B6BEE1571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>41</c:v>
@@ -917,69 +917,69 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45719</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45663</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>306</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>301</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>289</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>284</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>273</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256</c:v>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45719</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45670</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45663</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,7 +1130,7 @@
                   <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>267</c:v>
@@ -1139,19 +1139,19 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>262</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>245</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>41</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="D72" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N73" sqref="N73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4853,6 +4853,20 @@
       </c>
       <c r="C7">
         <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="1">
+        <v>45719</v>
+      </c>
+      <c r="D18">
+        <v>308</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45719</v>
+      </c>
+      <c r="G18">
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/3/9 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09D81B1-30A7-40CF-BDA7-D06B6BEE1571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097559B9-84BC-43D6-B942-859EF5BADD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45726</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45670</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$26</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>306</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>301</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>289</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>284</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>273</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,54 +1086,54 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45726</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45677</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45670</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$26</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>267</c:v>
@@ -1142,13 +1142,13 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>262</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>250</c:v>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="310"/>
+          <c:max val="320"/>
           <c:min val="240"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1621,7 +1621,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4812,7 +4812,7 @@
   <dimension ref="B2:Q99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D72" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N73" sqref="N73"/>
+      <selection activeCell="M72" sqref="M72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <v>45726</v>
+      </c>
+      <c r="D17">
+        <v>309</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45726</v>
+      </c>
+      <c r="G17">
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/3/21 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097559B9-84BC-43D6-B942-859EF5BADD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C93D09-0422-40F9-83E9-E8CD0E147DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45733</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45677</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$16:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>309</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>306</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>301</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>289</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>284</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>264</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,57 +1086,57 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45733</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45684</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45677</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$16:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>267</c:v>
@@ -1145,13 +1145,13 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>262</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D72" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M72" sqref="M72"/>
+    <sheetView tabSelected="1" topLeftCell="D73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4821,25 +4821,25 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4847,12 +4847,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>49</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>45733</v>
+      </c>
+      <c r="D16">
+        <v>310</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45733</v>
+      </c>
+      <c r="G16">
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/3/24 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C93D09-0422-40F9-83E9-E8CD0E147DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65975AF8-0AFF-4EA1-B10D-21B8914EB132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>51</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45740</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45684</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45677</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$24</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>309</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>306</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>301</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>289</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>284</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45740</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45691</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45684</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45677</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$24</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,16 +1130,16 @@
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>267</c:v>
@@ -1148,10 +1148,10 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>262</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>254</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>51</c:v>
@@ -4223,13 +4223,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4259,13 +4259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,10 +4809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q99"/>
+  <dimension ref="B2:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
+    <sheetView tabSelected="1" topLeftCell="D63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4821,33 +4821,33 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -4855,770 +4855,736 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
-        <v>45733</v>
-      </c>
-      <c r="D16">
-        <v>310</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45733</v>
-      </c>
-      <c r="G16">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>45726</v>
-      </c>
-      <c r="D17">
-        <v>309</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45726</v>
-      </c>
-      <c r="G17">
-        <v>294</v>
-      </c>
-    </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C18" s="1">
-        <v>45719</v>
+        <v>45740</v>
       </c>
       <c r="D18">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="F18" s="1">
-        <v>45719</v>
+        <v>45740</v>
       </c>
       <c r="G18">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
-        <v>45712</v>
+        <v>45733</v>
       </c>
       <c r="D19">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="F19" s="1">
-        <v>45712</v>
+        <v>45733</v>
       </c>
       <c r="G19">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
-        <v>45705</v>
+        <v>45726</v>
       </c>
       <c r="D20">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="F20" s="1">
-        <v>45705</v>
+        <v>45726</v>
       </c>
       <c r="G20">
-        <v>267</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
-        <v>45698</v>
+        <v>45719</v>
       </c>
       <c r="D21">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="F21" s="1">
-        <v>45698</v>
+        <v>45719</v>
       </c>
       <c r="G21">
-        <v>267</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
-        <v>45691</v>
+        <v>45712</v>
       </c>
       <c r="D22">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="F22" s="1">
-        <v>45691</v>
+        <v>45712</v>
       </c>
       <c r="G22">
-        <v>267</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
-        <v>45684</v>
+        <v>45705</v>
       </c>
       <c r="D23">
-        <v>284</v>
+        <v>301</v>
       </c>
       <c r="F23" s="1">
-        <v>45684</v>
+        <v>45705</v>
       </c>
       <c r="G23">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
-        <v>45677</v>
+        <v>45698</v>
       </c>
       <c r="D24">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="F24" s="1">
-        <v>45677</v>
+        <v>45698</v>
       </c>
       <c r="G24">
-        <v>254</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
-        <v>45670</v>
+        <v>45691</v>
       </c>
       <c r="D25">
-        <v>264</v>
+        <v>289</v>
       </c>
       <c r="F25" s="1">
-        <v>45670</v>
+        <v>45691</v>
       </c>
       <c r="G25">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>45663</v>
+        <v>45684</v>
       </c>
       <c r="D26">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="F26" s="1">
-        <v>45663</v>
+        <v>45684</v>
       </c>
       <c r="G26">
-        <v>250</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>45642</v>
+        <v>45677</v>
       </c>
       <c r="D27">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="F27" s="1">
-        <v>45642</v>
+        <v>45677</v>
       </c>
       <c r="G27">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>45635</v>
+        <v>45670</v>
       </c>
       <c r="D28">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="F28" s="1">
-        <v>45635</v>
+        <v>45670</v>
       </c>
       <c r="G28">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>45628</v>
+        <v>45663</v>
       </c>
       <c r="D29">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="F29" s="1">
-        <v>45628</v>
+        <v>45663</v>
       </c>
       <c r="G29">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>45621</v>
+        <v>45642</v>
       </c>
       <c r="D30">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="F30" s="1">
-        <v>45621</v>
+        <v>45642</v>
       </c>
       <c r="G30">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>45614</v>
+        <v>45635</v>
       </c>
       <c r="D31">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="F31" s="1">
-        <v>45614</v>
+        <v>45635</v>
       </c>
       <c r="G31">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>45607</v>
+        <v>45628</v>
       </c>
       <c r="D32">
+        <v>251</v>
+      </c>
+      <c r="F32" s="1">
+        <v>45628</v>
+      </c>
+      <c r="G32">
         <v>239</v>
-      </c>
-      <c r="F32" s="1">
-        <v>45607</v>
-      </c>
-      <c r="G32">
-        <v>230</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>45600</v>
+        <v>45621</v>
       </c>
       <c r="D33">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F33" s="1">
-        <v>45600</v>
+        <v>45621</v>
       </c>
       <c r="G33">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
-        <v>45579</v>
+        <v>45614</v>
       </c>
       <c r="D34">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="F34" s="1">
-        <v>45579</v>
+        <v>45614</v>
       </c>
       <c r="G34">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
-        <v>45572</v>
+        <v>45607</v>
       </c>
       <c r="D35">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="F35" s="1">
-        <v>45572</v>
+        <v>45607</v>
       </c>
       <c r="G35">
-        <v>216</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>45565</v>
+        <v>45600</v>
       </c>
       <c r="D36">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="F36" s="1">
-        <v>45565</v>
+        <v>45600</v>
       </c>
       <c r="G36">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
-        <v>45537</v>
+        <v>45579</v>
       </c>
       <c r="D37">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="F37" s="1">
-        <v>45537</v>
+        <v>45579</v>
       </c>
       <c r="G37">
-        <v>207</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
-        <v>45530</v>
+        <v>45572</v>
       </c>
       <c r="D38">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="F38" s="1">
-        <v>45530</v>
+        <v>45572</v>
       </c>
       <c r="G38">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
-        <v>45523</v>
+        <v>45565</v>
       </c>
       <c r="D39">
+        <v>223</v>
+      </c>
+      <c r="F39" s="1">
+        <v>45565</v>
+      </c>
+      <c r="G39">
         <v>216</v>
-      </c>
-      <c r="F39" s="1">
-        <v>45523</v>
-      </c>
-      <c r="G39">
-        <v>200</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
-        <v>45516</v>
+        <v>45537</v>
       </c>
       <c r="D40">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="F40" s="1">
-        <v>45516</v>
+        <v>45537</v>
       </c>
       <c r="G40">
-        <v>190</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <v>45509</v>
+        <v>45530</v>
       </c>
       <c r="D41">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="F41" s="1">
-        <v>45509</v>
+        <v>45530</v>
       </c>
       <c r="G41">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
-        <v>45502</v>
+        <v>45523</v>
       </c>
       <c r="D42">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="F42" s="1">
-        <v>45502</v>
+        <v>45523</v>
       </c>
       <c r="G42">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
-        <v>45495</v>
+        <v>45516</v>
       </c>
       <c r="D43">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="F43" s="1">
-        <v>45495</v>
+        <v>45516</v>
       </c>
       <c r="G43">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
-        <v>45488</v>
+        <v>45509</v>
       </c>
       <c r="D44">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="F44" s="1">
-        <v>45488</v>
+        <v>45509</v>
       </c>
       <c r="G44">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
-        <v>45481</v>
+        <v>45502</v>
       </c>
       <c r="D45">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="F45" s="1">
-        <v>45481</v>
+        <v>45502</v>
       </c>
       <c r="G45">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
-        <v>45474</v>
+        <v>45495</v>
       </c>
       <c r="D46">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="F46" s="1">
-        <v>45474</v>
+        <v>45495</v>
       </c>
       <c r="G46">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
-        <v>45467</v>
+        <v>45488</v>
       </c>
       <c r="D47">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="F47" s="1">
-        <v>45467</v>
+        <v>45488</v>
       </c>
       <c r="G47">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
-        <v>45460</v>
+        <v>45481</v>
       </c>
       <c r="D48">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F48" s="1">
-        <v>45460</v>
+        <v>45481</v>
       </c>
       <c r="G48">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
-        <v>45453</v>
+        <v>45474</v>
       </c>
       <c r="D49">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="F49" s="1">
-        <v>45453</v>
+        <v>45474</v>
       </c>
       <c r="G49">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
-        <v>45446</v>
+        <v>45467</v>
       </c>
       <c r="D50">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="F50" s="1">
-        <v>45446</v>
+        <v>45467</v>
       </c>
       <c r="G50">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
-        <v>45439</v>
+        <v>45460</v>
       </c>
       <c r="D51">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F51" s="1">
-        <v>45439</v>
+        <v>45460</v>
       </c>
       <c r="G51">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
-        <v>45432</v>
+        <v>45453</v>
       </c>
       <c r="D52">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F52" s="1">
-        <v>45432</v>
+        <v>45453</v>
       </c>
       <c r="G52">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
-        <v>45425</v>
+        <v>45446</v>
       </c>
       <c r="D53">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F53" s="1">
-        <v>45425</v>
+        <v>45446</v>
       </c>
       <c r="G53">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
-        <v>45418</v>
+        <v>45439</v>
       </c>
       <c r="D54">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F54" s="1">
-        <v>45418</v>
+        <v>45439</v>
       </c>
       <c r="G54">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
-        <v>45411</v>
+        <v>45432</v>
       </c>
       <c r="D55">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F55" s="1">
-        <v>45411</v>
+        <v>45432</v>
       </c>
       <c r="G55">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
-        <v>45404</v>
+        <v>45425</v>
       </c>
       <c r="D56">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F56" s="1">
-        <v>45404</v>
+        <v>45425</v>
       </c>
       <c r="G56">
-        <v>141</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
-        <v>45397</v>
+        <v>45418</v>
       </c>
       <c r="D57">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="F57" s="1">
-        <v>45397</v>
+        <v>45418</v>
       </c>
       <c r="G57">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
-        <v>45390</v>
+        <v>45411</v>
       </c>
       <c r="D58">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="F58" s="1">
-        <v>45390</v>
+        <v>45411</v>
       </c>
       <c r="G58">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
-        <v>45383</v>
+        <v>45404</v>
       </c>
       <c r="D59">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="F59" s="1">
-        <v>45383</v>
+        <v>45404</v>
       </c>
       <c r="G59">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
-        <v>45376</v>
+        <v>45397</v>
       </c>
       <c r="D60">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="F60" s="1">
-        <v>45376</v>
+        <v>45397</v>
       </c>
       <c r="G60">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
-        <v>45369</v>
+        <v>45390</v>
       </c>
       <c r="D61">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="F61" s="1">
-        <v>45369</v>
+        <v>45390</v>
       </c>
       <c r="G61">
-        <v>97</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
-        <v>45362</v>
+        <v>45383</v>
       </c>
       <c r="D62">
-        <v>113</v>
-      </c>
-      <c r="F62" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="F62" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G62">
+        <v>119</v>
+      </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
-        <v>45355</v>
+        <v>45376</v>
       </c>
       <c r="D63">
-        <v>108</v>
+        <v>129</v>
+      </c>
+      <c r="F63" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G63">
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
-        <v>45348</v>
+        <v>45369</v>
       </c>
       <c r="D64">
-        <v>102</v>
+        <v>123</v>
+      </c>
+      <c r="F64" s="1">
+        <v>45369</v>
+      </c>
+      <c r="G64">
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
-        <v>45341</v>
+        <v>45362</v>
       </c>
       <c r="D65">
-        <v>95</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F65" s="1"/>
     </row>
     <row r="66" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
-        <v>45334</v>
+        <v>45355</v>
       </c>
       <c r="D66">
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
-        <v>45327</v>
+        <v>45348</v>
       </c>
       <c r="D67">
-        <v>66</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
-        <v>45320</v>
+        <v>45341</v>
       </c>
       <c r="D68">
-        <v>55</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
-        <v>45313</v>
+        <v>45334</v>
       </c>
       <c r="D69">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
+        <v>45327</v>
+      </c>
+      <c r="D70">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C71" s="1">
+        <v>45320</v>
+      </c>
+      <c r="D71">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C72" s="1">
+        <v>45313</v>
+      </c>
+      <c r="D72">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C73" s="1">
         <v>45306</v>
       </c>
-      <c r="D70">
+      <c r="D73">
         <v>52</v>
       </c>
-    </row>
-    <row r="74" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
-      <c r="L74" s="2"/>
-      <c r="M74" s="2"/>
-      <c r="N74" s="2"/>
-      <c r="O74" s="2"/>
-      <c r="P74" s="2"/>
-      <c r="Q74" s="2"/>
-    </row>
-    <row r="75" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
-      <c r="L75" s="2"/>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
-      <c r="O75" s="2"/>
-      <c r="P75" s="2"/>
-      <c r="Q75" s="2"/>
-    </row>
-    <row r="76" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2"/>
-      <c r="O76" s="2"/>
-      <c r="P76" s="2"/>
-      <c r="Q76" s="2"/>
     </row>
     <row r="77" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D77" s="2"/>
@@ -5988,9 +5954,57 @@
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
     </row>
+    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
+      <c r="L100" s="2"/>
+      <c r="M100" s="2"/>
+      <c r="N100" s="2"/>
+      <c r="O100" s="2"/>
+      <c r="P100" s="2"/>
+      <c r="Q100" s="2"/>
+    </row>
+    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
+      <c r="O101" s="2"/>
+      <c r="P101" s="2"/>
+      <c r="Q101" s="2"/>
+    </row>
+    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D74:Q99"/>
+    <mergeCell ref="D77:Q102"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/3/29 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65975AF8-0AFF-4EA1-B10D-21B8914EB132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6AF56C-A20A-470C-8FF0-3EAD54AF3254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45747</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45691</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$26</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>316</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>309</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>306</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>301</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>289</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,63 +1086,63 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45747</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45698</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45691</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$26</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>267</c:v>
@@ -1151,7 +1151,7 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>262</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L75" sqref="L75"/>
+    <sheetView tabSelected="1" topLeftCell="D74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M76" sqref="M76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>51</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <v>45747</v>
+      </c>
+      <c r="D17">
+        <v>317</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45747</v>
+      </c>
+      <c r="G17">
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/3/30 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6AF56C-A20A-470C-8FF0-3EAD54AF3254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE35192B-BDA8-4EE8-B56C-B258523E1D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>317</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>316</c:v>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="320"/>
-          <c:min val="240"/>
+          <c:max val="330"/>
+          <c:min val="260"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M76" sqref="M76"/>
+    <sheetView tabSelected="1" topLeftCell="D76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4860,7 +4860,7 @@
         <v>45747</v>
       </c>
       <c r="D17">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="F17" s="1">
         <v>45747</v>

</xml_diff>

<commit_message>
LGHUB 2025/4/3 更新 1 (完)
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE35192B-BDA8-4EE8-B56C-B258523E1D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD7FD3C-E31B-46AE-8433-17B576C47056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>323</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>316</c:v>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -4812,7 +4812,7 @@
   <dimension ref="B2:Q102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L75" sqref="L75"/>
+      <selection activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4860,7 +4860,7 @@
         <v>45747</v>
       </c>
       <c r="D17">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F17" s="1">
         <v>45747</v>

</xml_diff>

<commit_message>
LGHUB 2025/4/7 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD7FD3C-E31B-46AE-8433-17B576C47056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501610D6-0C98-4BB3-9839-A016B10A3D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,7 +577,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>57</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45754</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45698</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45691</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$16:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>325</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>316</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>309</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>306</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>301</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>295</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45754</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45705</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45698</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45691</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$16:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,22 +1130,22 @@
                   <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>267</c:v>
@@ -1797,7 +1797,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>57</c:v>
@@ -4821,17 +4821,17 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -4839,20 +4839,34 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
         <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>45754</v>
+      </c>
+      <c r="D16">
+        <v>327</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45754</v>
+      </c>
+      <c r="G16">
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/4/10 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501610D6-0C98-4BB3-9839-A016B10A3D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D2A9DC-95BC-4475-8218-E3281470D948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>327</c:v>
+                  <c:v>330</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>325</c:v>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -4812,7 +4812,7 @@
   <dimension ref="B2:Q102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L76" sqref="L76"/>
+      <selection activeCell="M76" sqref="M76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
@@ -4860,7 +4860,7 @@
         <v>45754</v>
       </c>
       <c r="D16">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="F16" s="1">
         <v>45754</v>

</xml_diff>

<commit_message>
LGHUB 2025/4/17 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D2A9DC-95BC-4475-8218-E3281470D948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2C58D4-7D40-4BFB-96C3-D2311294AB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45761</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45705</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$24</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>325</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>316</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>309</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>306</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,69 +1086,69 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45761</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45712</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45705</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$24</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>302</c:v>
+                  <c:v>303</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>267</c:v>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="330"/>
+          <c:max val="340"/>
           <c:min val="260"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4223,13 +4223,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4259,13 +4259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,10 +4809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q102"/>
+  <dimension ref="B2:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M76" sqref="M76"/>
+    <sheetView tabSelected="1" topLeftCell="D79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4821,862 +4821,812 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
-        <v>45754</v>
-      </c>
-      <c r="D16">
-        <v>330</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45754</v>
-      </c>
-      <c r="G16">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>45747</v>
-      </c>
-      <c r="D17">
-        <v>325</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45747</v>
-      </c>
-      <c r="G17">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="1">
-        <v>45740</v>
-      </c>
-      <c r="D18">
-        <v>316</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45740</v>
-      </c>
-      <c r="G18">
-        <v>296</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
-        <v>45733</v>
+        <v>45761</v>
       </c>
       <c r="D19">
-        <v>310</v>
+        <v>334</v>
       </c>
       <c r="F19" s="1">
-        <v>45733</v>
+        <v>45761</v>
       </c>
       <c r="G19">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
-        <v>45726</v>
+        <v>45754</v>
       </c>
       <c r="D20">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="F20" s="1">
-        <v>45726</v>
+        <v>45754</v>
       </c>
       <c r="G20">
-        <v>294</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
-        <v>45719</v>
+        <v>45747</v>
       </c>
       <c r="D21">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="F21" s="1">
-        <v>45719</v>
+        <v>45747</v>
       </c>
       <c r="G21">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
-        <v>45712</v>
+        <v>45740</v>
       </c>
       <c r="D22">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="F22" s="1">
-        <v>45712</v>
+        <v>45740</v>
       </c>
       <c r="G22">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
-        <v>45705</v>
+        <v>45733</v>
       </c>
       <c r="D23">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="F23" s="1">
-        <v>45705</v>
+        <v>45733</v>
       </c>
       <c r="G23">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
-        <v>45698</v>
+        <v>45726</v>
       </c>
       <c r="D24">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="F24" s="1">
-        <v>45698</v>
+        <v>45726</v>
       </c>
       <c r="G24">
-        <v>267</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
-        <v>45691</v>
+        <v>45719</v>
       </c>
       <c r="D25">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="F25" s="1">
-        <v>45691</v>
+        <v>45719</v>
       </c>
       <c r="G25">
-        <v>267</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>45684</v>
+        <v>45712</v>
       </c>
       <c r="D26">
-        <v>284</v>
+        <v>306</v>
       </c>
       <c r="F26" s="1">
-        <v>45684</v>
+        <v>45712</v>
       </c>
       <c r="G26">
-        <v>262</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>45677</v>
+        <v>45705</v>
       </c>
       <c r="D27">
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="F27" s="1">
-        <v>45677</v>
+        <v>45705</v>
       </c>
       <c r="G27">
-        <v>254</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>45670</v>
+        <v>45698</v>
       </c>
       <c r="D28">
-        <v>264</v>
+        <v>295</v>
       </c>
       <c r="F28" s="1">
-        <v>45670</v>
+        <v>45698</v>
       </c>
       <c r="G28">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>45663</v>
+        <v>45691</v>
       </c>
       <c r="D29">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="F29" s="1">
-        <v>45663</v>
+        <v>45691</v>
       </c>
       <c r="G29">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>45642</v>
+        <v>45684</v>
       </c>
       <c r="D30">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="F30" s="1">
-        <v>45642</v>
+        <v>45684</v>
       </c>
       <c r="G30">
-        <v>245</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>45635</v>
+        <v>45677</v>
       </c>
       <c r="D31">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="F31" s="1">
-        <v>45635</v>
+        <v>45677</v>
       </c>
       <c r="G31">
-        <v>243</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>45628</v>
+        <v>45670</v>
       </c>
       <c r="D32">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="F32" s="1">
-        <v>45628</v>
+        <v>45670</v>
       </c>
       <c r="G32">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>45621</v>
+        <v>45663</v>
       </c>
       <c r="D33">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="F33" s="1">
-        <v>45621</v>
+        <v>45663</v>
       </c>
       <c r="G33">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
-        <v>45614</v>
+        <v>45642</v>
       </c>
       <c r="D34">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F34" s="1">
-        <v>45614</v>
+        <v>45642</v>
       </c>
       <c r="G34">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
-        <v>45607</v>
+        <v>45635</v>
       </c>
       <c r="D35">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="F35" s="1">
-        <v>45607</v>
+        <v>45635</v>
       </c>
       <c r="G35">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>45600</v>
+        <v>45628</v>
       </c>
       <c r="D36">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F36" s="1">
-        <v>45600</v>
+        <v>45628</v>
       </c>
       <c r="G36">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
-        <v>45579</v>
+        <v>45621</v>
       </c>
       <c r="D37">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="F37" s="1">
-        <v>45579</v>
+        <v>45621</v>
       </c>
       <c r="G37">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
-        <v>45572</v>
+        <v>45614</v>
       </c>
       <c r="D38">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="F38" s="1">
-        <v>45572</v>
+        <v>45614</v>
       </c>
       <c r="G38">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
-        <v>45565</v>
+        <v>45607</v>
       </c>
       <c r="D39">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="F39" s="1">
-        <v>45565</v>
+        <v>45607</v>
       </c>
       <c r="G39">
-        <v>216</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
-        <v>45537</v>
+        <v>45600</v>
       </c>
       <c r="D40">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="F40" s="1">
-        <v>45537</v>
+        <v>45600</v>
       </c>
       <c r="G40">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <v>45530</v>
+        <v>45579</v>
       </c>
       <c r="D41">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="F41" s="1">
-        <v>45530</v>
+        <v>45579</v>
       </c>
       <c r="G41">
-        <v>207</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
-        <v>45523</v>
+        <v>45572</v>
       </c>
       <c r="D42">
+        <v>227</v>
+      </c>
+      <c r="F42" s="1">
+        <v>45572</v>
+      </c>
+      <c r="G42">
         <v>216</v>
-      </c>
-      <c r="F42" s="1">
-        <v>45523</v>
-      </c>
-      <c r="G42">
-        <v>200</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
-        <v>45516</v>
+        <v>45565</v>
       </c>
       <c r="D43">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="F43" s="1">
-        <v>45516</v>
+        <v>45565</v>
       </c>
       <c r="G43">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
-        <v>45509</v>
+        <v>45537</v>
       </c>
       <c r="D44">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F44" s="1">
-        <v>45509</v>
+        <v>45537</v>
       </c>
       <c r="G44">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
-        <v>45502</v>
+        <v>45530</v>
       </c>
       <c r="D45">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="F45" s="1">
-        <v>45502</v>
+        <v>45530</v>
       </c>
       <c r="G45">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
-        <v>45495</v>
+        <v>45523</v>
       </c>
       <c r="D46">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="F46" s="1">
-        <v>45495</v>
+        <v>45523</v>
       </c>
       <c r="G46">
-        <v>183</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
-        <v>45488</v>
+        <v>45516</v>
       </c>
       <c r="D47">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="F47" s="1">
-        <v>45488</v>
+        <v>45516</v>
       </c>
       <c r="G47">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
-        <v>45481</v>
+        <v>45509</v>
       </c>
       <c r="D48">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="F48" s="1">
-        <v>45481</v>
+        <v>45509</v>
       </c>
       <c r="G48">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
-        <v>45474</v>
+        <v>45502</v>
       </c>
       <c r="D49">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F49" s="1">
-        <v>45474</v>
+        <v>45502</v>
       </c>
       <c r="G49">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
-        <v>45467</v>
+        <v>45495</v>
       </c>
       <c r="D50">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="F50" s="1">
-        <v>45467</v>
+        <v>45495</v>
       </c>
       <c r="G50">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
-        <v>45460</v>
+        <v>45488</v>
       </c>
       <c r="D51">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="F51" s="1">
-        <v>45460</v>
+        <v>45488</v>
       </c>
       <c r="G51">
-        <v>165</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
-        <v>45453</v>
+        <v>45481</v>
       </c>
       <c r="D52">
+        <v>188</v>
+      </c>
+      <c r="F52" s="1">
+        <v>45481</v>
+      </c>
+      <c r="G52">
         <v>180</v>
-      </c>
-      <c r="F52" s="1">
-        <v>45453</v>
-      </c>
-      <c r="G52">
-        <v>164</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="D53">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="F53" s="1">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="G53">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
-        <v>45439</v>
+        <v>45467</v>
       </c>
       <c r="D54">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F54" s="1">
-        <v>45439</v>
+        <v>45467</v>
       </c>
       <c r="G54">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
-        <v>45432</v>
+        <v>45460</v>
       </c>
       <c r="D55">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="F55" s="1">
-        <v>45432</v>
+        <v>45460</v>
       </c>
       <c r="G55">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
-        <v>45425</v>
+        <v>45453</v>
       </c>
       <c r="D56">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F56" s="1">
-        <v>45425</v>
+        <v>45453</v>
       </c>
       <c r="G56">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
-        <v>45418</v>
+        <v>45446</v>
       </c>
       <c r="D57">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F57" s="1">
-        <v>45418</v>
+        <v>45446</v>
       </c>
       <c r="G57">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
-        <v>45411</v>
+        <v>45439</v>
       </c>
       <c r="D58">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F58" s="1">
-        <v>45411</v>
+        <v>45439</v>
       </c>
       <c r="G58">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
-        <v>45404</v>
+        <v>45432</v>
       </c>
       <c r="D59">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F59" s="1">
-        <v>45404</v>
+        <v>45432</v>
       </c>
       <c r="G59">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
-        <v>45397</v>
+        <v>45425</v>
       </c>
       <c r="D60">
+        <v>170</v>
+      </c>
+      <c r="F60" s="1">
+        <v>45425</v>
+      </c>
+      <c r="G60">
         <v>157</v>
-      </c>
-      <c r="F60" s="1">
-        <v>45397</v>
-      </c>
-      <c r="G60">
-        <v>132</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
-        <v>45390</v>
+        <v>45418</v>
       </c>
       <c r="D61">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="F61" s="1">
-        <v>45390</v>
+        <v>45418</v>
       </c>
       <c r="G61">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
-        <v>45383</v>
+        <v>45411</v>
       </c>
       <c r="D62">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="F62" s="1">
-        <v>45383</v>
+        <v>45411</v>
       </c>
       <c r="G62">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
-        <v>45376</v>
+        <v>45404</v>
       </c>
       <c r="D63">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="F63" s="1">
-        <v>45376</v>
+        <v>45404</v>
       </c>
       <c r="G63">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
+        <v>45397</v>
+      </c>
+      <c r="D64">
+        <v>157</v>
+      </c>
+      <c r="F64" s="1">
+        <v>45397</v>
+      </c>
+      <c r="G64">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C65" s="1">
+        <v>45390</v>
+      </c>
+      <c r="D65">
+        <v>146</v>
+      </c>
+      <c r="F65" s="1">
+        <v>45390</v>
+      </c>
+      <c r="G65">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C66" s="1">
+        <v>45383</v>
+      </c>
+      <c r="D66">
+        <v>138</v>
+      </c>
+      <c r="F66" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G66">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C67" s="1">
+        <v>45376</v>
+      </c>
+      <c r="D67">
+        <v>129</v>
+      </c>
+      <c r="F67" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G67">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C68" s="1">
         <v>45369</v>
       </c>
-      <c r="D64">
+      <c r="D68">
         <v>123</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F68" s="1">
         <v>45369</v>
       </c>
-      <c r="G64">
+      <c r="G68">
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C65" s="1">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C69" s="1">
         <v>45362</v>
       </c>
-      <c r="D65">
+      <c r="D69">
         <v>113</v>
       </c>
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C66" s="1">
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C70" s="1">
         <v>45355</v>
       </c>
-      <c r="D66">
+      <c r="D70">
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C67" s="1">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C71" s="1">
         <v>45348</v>
       </c>
-      <c r="D67">
+      <c r="D71">
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C68" s="1">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C72" s="1">
         <v>45341</v>
       </c>
-      <c r="D68">
+      <c r="D72">
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C69" s="1">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C73" s="1">
         <v>45334</v>
       </c>
-      <c r="D69">
+      <c r="D73">
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C70" s="1">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C74" s="1">
         <v>45327</v>
       </c>
-      <c r="D70">
+      <c r="D74">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C71" s="1">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C75" s="1">
         <v>45320</v>
       </c>
-      <c r="D71">
+      <c r="D75">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C72" s="1">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C76" s="1">
         <v>45313</v>
       </c>
-      <c r="D72">
+      <c r="D76">
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="C73" s="1">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C77" s="1">
         <v>45306</v>
       </c>
-      <c r="D73">
+      <c r="D77">
         <v>52</v>
       </c>
-    </row>
-    <row r="77" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
-      <c r="L77" s="2"/>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="2"/>
-    </row>
-    <row r="78" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
-      <c r="Q78" s="2"/>
-    </row>
-    <row r="79" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
-      <c r="O79" s="2"/>
-      <c r="P79" s="2"/>
-      <c r="Q79" s="2"/>
-    </row>
-    <row r="80" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
-      <c r="O80" s="2"/>
-      <c r="P80" s="2"/>
-      <c r="Q80" s="2"/>
     </row>
     <row r="81" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D81" s="2"/>
@@ -6030,9 +5980,73 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
+    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+      <c r="L103" s="2"/>
+      <c r="M103" s="2"/>
+      <c r="N103" s="2"/>
+      <c r="O103" s="2"/>
+      <c r="P103" s="2"/>
+      <c r="Q103" s="2"/>
+    </row>
+    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+      <c r="L104" s="2"/>
+      <c r="M104" s="2"/>
+      <c r="N104" s="2"/>
+      <c r="O104" s="2"/>
+      <c r="P104" s="2"/>
+      <c r="Q104" s="2"/>
+    </row>
+    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+      <c r="L105" s="2"/>
+      <c r="M105" s="2"/>
+      <c r="N105" s="2"/>
+      <c r="O105" s="2"/>
+      <c r="P105" s="2"/>
+      <c r="Q105" s="2"/>
+    </row>
+    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+      <c r="L106" s="2"/>
+      <c r="M106" s="2"/>
+      <c r="N106" s="2"/>
+      <c r="O106" s="2"/>
+      <c r="P106" s="2"/>
+      <c r="Q106" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D77:Q102"/>
+    <mergeCell ref="D81:Q106"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/4/20 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2C58D4-7D40-4BFB-96C3-D2311294AB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE2984A-92B7-4239-B178-12B097D62775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>58</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45768</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45712</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>334</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>325</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>316</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>309</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>306</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45768</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45719</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45712</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,28 +1130,28 @@
                   <c:v>303</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>302</c:v>
+                  <c:v>303</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>267</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>58</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L80" sqref="L80"/>
+    <sheetView tabSelected="1" topLeftCell="D78" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4853,6 +4853,20 @@
       </c>
       <c r="C7">
         <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="1">
+        <v>45768</v>
+      </c>
+      <c r="D18">
+        <v>338</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45768</v>
+      </c>
+      <c r="G18">
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/4/24 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE2984A-92B7-4239-B178-12B097D62775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F3C4C7-CCE8-440E-AC34-537C6DFFC464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>303</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>303</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D78" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K80" sqref="K80"/>
+    <sheetView tabSelected="1" topLeftCell="D80" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">
@@ -4866,7 +4866,7 @@
         <v>45768</v>
       </c>
       <c r="G18">
-        <v>303</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/4/26 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F3C4C7-CCE8-440E-AC34-537C6DFFC464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D0AEEE-4459-4F98-BCAE-777A98ECCB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>338</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>334</c:v>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="340"/>
-          <c:min val="260"/>
+          <c:max val="350"/>
+          <c:min val="280"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D80" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="D79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">
@@ -4860,7 +4860,7 @@
         <v>45768</v>
       </c>
       <c r="D18">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="F18" s="1">
         <v>45768</v>

</xml_diff>

<commit_message>
LGHUB 2025/4/28 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D0AEEE-4459-4F98-BCAE-777A98ECCB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FE6CF0-C41E-4943-8633-BB71A6F049E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45775</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45719</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$26</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>343</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>334</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>325</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>316</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>309</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>308</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>306</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,69 +1086,69 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45775</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45726</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45719</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$26</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>319</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>286</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K80" sqref="K80"/>
+    <sheetView tabSelected="1" topLeftCell="D71" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>73</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <v>45775</v>
+      </c>
+      <c r="D17">
+        <v>346</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45775</v>
+      </c>
+      <c r="G17">
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/5/1 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FE6CF0-C41E-4943-8633-BB71A6F049E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF9087D-B8DB-4A17-9F9D-7AADD476E9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>346</c:v>
+                  <c:v>348</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>343</c:v>
@@ -1529,7 +1529,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>(1</a:t>
+              <a:t>(5</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -1555,7 +1555,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>- 4</a:t>
+              <a:t>- 8</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D71" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L80" sqref="L80"/>
+    <sheetView tabSelected="1" topLeftCell="D79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">
@@ -4860,7 +4860,7 @@
         <v>45775</v>
       </c>
       <c r="D17">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F17" s="1">
         <v>45775</v>

</xml_diff>

<commit_message>
LGHUB 2025/5/4 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF9087D-B8DB-4A17-9F9D-7AADD476E9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A8E402-7651-40E6-BB59-3DFD7053A152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45782</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45726</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$16:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>348</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>343</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>334</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>325</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>316</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>309</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>308</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45782</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45733</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45726</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$16:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,28 +1130,28 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>319</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>286</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="350"/>
-          <c:min val="280"/>
+          <c:max val="360"/>
+          <c:min val="290"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4821,38 +4821,52 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>45782</v>
+      </c>
+      <c r="D16">
+        <v>355</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45782</v>
+      </c>
+      <c r="G16">
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/5/5 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A8E402-7651-40E6-BB59-3DFD7053A152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5E196F-6D60-4F2B-ABFD-A35FE8250531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,7 +577,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>355</c:v>
+                  <c:v>356</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>348</c:v>
@@ -1797,7 +1797,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4812,7 +4812,7 @@
   <dimension ref="B2:Q106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K80" sqref="K80"/>
+      <selection activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
@@ -4860,7 +4860,7 @@
         <v>45782</v>
       </c>
       <c r="D16">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F16" s="1">
         <v>45782</v>

</xml_diff>

<commit_message>
LGHUB 2025/5/10 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5E196F-6D60-4F2B-ABFD-A35FE8250531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CAA3EE-2AC7-4AFD-943A-6B4580BF7CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45789</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45733</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$24</c:f>
+              <c:f>Sheet1!$D$20:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>356</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>348</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>343</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>334</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>325</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>316</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>309</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45789</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45740</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45733</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$24</c:f>
+              <c:f>Sheet1!$G$20:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1133,25 +1133,25 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>319</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -4223,13 +4223,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4259,13 +4259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,10 +4809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q106"/>
+  <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L80" sqref="L80"/>
+    <sheetView tabSelected="1" topLeftCell="D83" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4821,25 +4821,25 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -4855,902 +4855,836 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
-        <v>45782</v>
-      </c>
-      <c r="D16">
-        <v>356</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45782</v>
-      </c>
-      <c r="G16">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>45775</v>
-      </c>
-      <c r="D17">
-        <v>348</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45775</v>
-      </c>
-      <c r="G17">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="1">
-        <v>45768</v>
-      </c>
-      <c r="D18">
-        <v>343</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45768</v>
-      </c>
-      <c r="G18">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="1">
-        <v>45761</v>
-      </c>
-      <c r="D19">
-        <v>334</v>
-      </c>
-      <c r="F19" s="1">
-        <v>45761</v>
-      </c>
-      <c r="G19">
-        <v>303</v>
-      </c>
-    </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
-        <v>45754</v>
+        <v>45789</v>
       </c>
       <c r="D20">
-        <v>330</v>
+        <v>359</v>
       </c>
       <c r="F20" s="1">
-        <v>45754</v>
+        <v>45789</v>
       </c>
       <c r="G20">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
-        <v>45747</v>
+        <v>45782</v>
       </c>
       <c r="D21">
-        <v>325</v>
+        <v>356</v>
       </c>
       <c r="F21" s="1">
-        <v>45747</v>
+        <v>45782</v>
       </c>
       <c r="G21">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
-        <v>45740</v>
+        <v>45775</v>
       </c>
       <c r="D22">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="F22" s="1">
-        <v>45740</v>
+        <v>45775</v>
       </c>
       <c r="G22">
-        <v>296</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
-        <v>45733</v>
+        <v>45768</v>
       </c>
       <c r="D23">
-        <v>310</v>
+        <v>343</v>
       </c>
       <c r="F23" s="1">
-        <v>45733</v>
+        <v>45768</v>
       </c>
       <c r="G23">
-        <v>296</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
-        <v>45726</v>
+        <v>45761</v>
       </c>
       <c r="D24">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="F24" s="1">
-        <v>45726</v>
+        <v>45761</v>
       </c>
       <c r="G24">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
-        <v>45719</v>
+        <v>45754</v>
       </c>
       <c r="D25">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="F25" s="1">
-        <v>45719</v>
+        <v>45754</v>
       </c>
       <c r="G25">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>45712</v>
+        <v>45747</v>
       </c>
       <c r="D26">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="F26" s="1">
-        <v>45712</v>
+        <v>45747</v>
       </c>
       <c r="G26">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>45705</v>
+        <v>45740</v>
       </c>
       <c r="D27">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="F27" s="1">
-        <v>45705</v>
+        <v>45740</v>
       </c>
       <c r="G27">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>45698</v>
+        <v>45733</v>
       </c>
       <c r="D28">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="F28" s="1">
-        <v>45698</v>
+        <v>45733</v>
       </c>
       <c r="G28">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>45691</v>
+        <v>45726</v>
       </c>
       <c r="D29">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="F29" s="1">
-        <v>45691</v>
+        <v>45726</v>
       </c>
       <c r="G29">
-        <v>267</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>45684</v>
+        <v>45719</v>
       </c>
       <c r="D30">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="F30" s="1">
-        <v>45684</v>
+        <v>45719</v>
       </c>
       <c r="G30">
-        <v>262</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>45677</v>
+        <v>45712</v>
       </c>
       <c r="D31">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="F31" s="1">
-        <v>45677</v>
+        <v>45712</v>
       </c>
       <c r="G31">
-        <v>254</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>45670</v>
+        <v>45705</v>
       </c>
       <c r="D32">
-        <v>264</v>
+        <v>301</v>
       </c>
       <c r="F32" s="1">
-        <v>45670</v>
+        <v>45705</v>
       </c>
       <c r="G32">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="D33">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="F33" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="G33">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
-        <v>45642</v>
+        <v>45691</v>
       </c>
       <c r="D34">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="F34" s="1">
-        <v>45642</v>
+        <v>45691</v>
       </c>
       <c r="G34">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
-        <v>45635</v>
+        <v>45684</v>
       </c>
       <c r="D35">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="F35" s="1">
-        <v>45635</v>
+        <v>45684</v>
       </c>
       <c r="G35">
-        <v>243</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="D36">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="F36" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="G36">
-        <v>239</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="D37">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="F37" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="G37">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="D38">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F38" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="G38">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="D39">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="F39" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="G39">
-        <v>230</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="D40">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F40" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="G40">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="D41">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="F41" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="G41">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="D42">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="F42" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="G42">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="D43">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="F43" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="G43">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="D44">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="F44" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="G44">
-        <v>207</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="D45">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="F45" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="G45">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="D46">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="F46" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="G46">
-        <v>200</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="D47">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="F47" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="G47">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="D48">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="F48" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="G48">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="D49">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F49" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="G49">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="D50">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="F50" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="G50">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="D51">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="F51" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="G51">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="D52">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="F52" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="G52">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="D53">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F53" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="G53">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="D54">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F54" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="G54">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="D55">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F55" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="G55">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="D56">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="F56" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="G56">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="D57">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F57" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="G57">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="D58">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F58" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="G58">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="D59">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F59" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="G59">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="D60">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="F60" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="G60">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="D61">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F61" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="G61">
-        <v>141</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="D62">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F62" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="G62">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="D63">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F63" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="G63">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="D64">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F64" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="G64">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
-        <v>45390</v>
+        <v>45425</v>
       </c>
       <c r="D65">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="F65" s="1">
-        <v>45390</v>
+        <v>45425</v>
       </c>
       <c r="G65">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
-        <v>45383</v>
+        <v>45418</v>
       </c>
       <c r="D66">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F66" s="1">
-        <v>45383</v>
+        <v>45418</v>
       </c>
       <c r="G66">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
-        <v>45376</v>
+        <v>45411</v>
       </c>
       <c r="D67">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="F67" s="1">
-        <v>45376</v>
+        <v>45411</v>
       </c>
       <c r="G67">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
-        <v>45369</v>
+        <v>45404</v>
       </c>
       <c r="D68">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="F68" s="1">
-        <v>45369</v>
+        <v>45404</v>
       </c>
       <c r="G68">
-        <v>97</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
-        <v>45362</v>
+        <v>45397</v>
       </c>
       <c r="D69">
-        <v>113</v>
-      </c>
-      <c r="F69" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="F69" s="1">
+        <v>45397</v>
+      </c>
+      <c r="G69">
+        <v>132</v>
+      </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
-        <v>45355</v>
+        <v>45390</v>
       </c>
       <c r="D70">
-        <v>108</v>
+        <v>146</v>
+      </c>
+      <c r="F70" s="1">
+        <v>45390</v>
+      </c>
+      <c r="G70">
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1">
-        <v>45348</v>
+        <v>45383</v>
       </c>
       <c r="D71">
-        <v>102</v>
+        <v>138</v>
+      </c>
+      <c r="F71" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G71">
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1">
-        <v>45341</v>
+        <v>45376</v>
       </c>
       <c r="D72">
-        <v>95</v>
+        <v>129</v>
+      </c>
+      <c r="F72" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G72">
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1">
-        <v>45334</v>
+        <v>45369</v>
       </c>
       <c r="D73">
-        <v>80</v>
+        <v>123</v>
+      </c>
+      <c r="F73" s="1">
+        <v>45369</v>
+      </c>
+      <c r="G73">
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1">
-        <v>45327</v>
+        <v>45362</v>
       </c>
       <c r="D74">
-        <v>66</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F74" s="1"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1">
-        <v>45320</v>
+        <v>45355</v>
       </c>
       <c r="D75">
-        <v>55</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1">
-        <v>45313</v>
+        <v>45348</v>
       </c>
       <c r="D76">
-        <v>53</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1">
+        <v>45341</v>
+      </c>
+      <c r="D77">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C78" s="1">
+        <v>45334</v>
+      </c>
+      <c r="D78">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C79" s="1">
+        <v>45327</v>
+      </c>
+      <c r="D79">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C80" s="1">
+        <v>45320</v>
+      </c>
+      <c r="D80">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C81" s="1">
+        <v>45313</v>
+      </c>
+      <c r="D81">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C82" s="1">
         <v>45306</v>
       </c>
-      <c r="D77">
+      <c r="D82">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
-      <c r="L81" s="2"/>
-      <c r="M81" s="2"/>
-      <c r="N81" s="2"/>
-      <c r="O81" s="2"/>
-      <c r="P81" s="2"/>
-      <c r="Q81" s="2"/>
-    </row>
-    <row r="82" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2"/>
-      <c r="N82" s="2"/>
-      <c r="O82" s="2"/>
-      <c r="P82" s="2"/>
-      <c r="Q82" s="2"/>
-    </row>
-    <row r="83" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
-      <c r="K83" s="2"/>
-      <c r="L83" s="2"/>
-      <c r="M83" s="2"/>
-      <c r="N83" s="2"/>
-      <c r="O83" s="2"/>
-      <c r="P83" s="2"/>
-      <c r="Q83" s="2"/>
-    </row>
-    <row r="84" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2"/>
-      <c r="N84" s="2"/>
-      <c r="O84" s="2"/>
-      <c r="P84" s="2"/>
-      <c r="Q84" s="2"/>
-    </row>
-    <row r="85" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
-      <c r="O85" s="2"/>
-      <c r="P85" s="2"/>
-      <c r="Q85" s="2"/>
-    </row>
-    <row r="86" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
@@ -5766,7 +5700,7 @@
       <c r="P86" s="2"/>
       <c r="Q86" s="2"/>
     </row>
-    <row r="87" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
@@ -5782,7 +5716,7 @@
       <c r="P87" s="2"/>
       <c r="Q87" s="2"/>
     </row>
-    <row r="88" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -5798,7 +5732,7 @@
       <c r="P88" s="2"/>
       <c r="Q88" s="2"/>
     </row>
-    <row r="89" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
@@ -5814,7 +5748,7 @@
       <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
     </row>
-    <row r="90" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
@@ -5830,7 +5764,7 @@
       <c r="P90" s="2"/>
       <c r="Q90" s="2"/>
     </row>
-    <row r="91" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -5846,7 +5780,7 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
     </row>
-    <row r="92" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
@@ -5862,7 +5796,7 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
     </row>
-    <row r="93" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -5878,7 +5812,7 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
     </row>
-    <row r="94" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -5894,7 +5828,7 @@
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
     </row>
-    <row r="95" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -5910,7 +5844,7 @@
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -6086,9 +6020,89 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
+    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+      <c r="K107" s="2"/>
+      <c r="L107" s="2"/>
+      <c r="M107" s="2"/>
+      <c r="N107" s="2"/>
+      <c r="O107" s="2"/>
+      <c r="P107" s="2"/>
+      <c r="Q107" s="2"/>
+    </row>
+    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+      <c r="L108" s="2"/>
+      <c r="M108" s="2"/>
+      <c r="N108" s="2"/>
+      <c r="O108" s="2"/>
+      <c r="P108" s="2"/>
+      <c r="Q108" s="2"/>
+    </row>
+    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+      <c r="M109" s="2"/>
+      <c r="N109" s="2"/>
+      <c r="O109" s="2"/>
+      <c r="P109" s="2"/>
+      <c r="Q109" s="2"/>
+    </row>
+    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+      <c r="L110" s="2"/>
+      <c r="M110" s="2"/>
+      <c r="N110" s="2"/>
+      <c r="O110" s="2"/>
+      <c r="P110" s="2"/>
+      <c r="Q110" s="2"/>
+    </row>
+    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+      <c r="L111" s="2"/>
+      <c r="M111" s="2"/>
+      <c r="N111" s="2"/>
+      <c r="O111" s="2"/>
+      <c r="P111" s="2"/>
+      <c r="Q111" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D81:Q106"/>
+    <mergeCell ref="D86:Q111"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/5/17 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD40ABC-21D1-4B3C-9A2F-4FDA512B9CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D7BA6A-F428-4986-B67A-47CA7A20F762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45796</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45740</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45733</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$20:$D$28</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>365</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>356</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>348</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>343</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>334</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>325</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>316</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>310</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,48 +1086,48 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45796</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45747</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45740</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45733</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$20:$G$28</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>320</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>320</c:v>
@@ -1136,19 +1136,19 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>319</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>296</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4812,7 +4812,7 @@
   <dimension ref="B2:Q111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+      <selection activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19" s="1">
+        <v>45796</v>
+      </c>
+      <c r="D19">
+        <v>366</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45796</v>
+      </c>
+      <c r="G19">
+        <v>349</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/5/24 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D7BA6A-F428-4986-B67A-47CA7A20F762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD26D54-A292-430A-A769-AE1B6A8B4DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45803</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45747</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45740</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>366</c:v>
+                  <c:v>379</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>365</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>356</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>348</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>343</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>334</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>316</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,51 +1086,51 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45803</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45754</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45747</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45740</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>349</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>320</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>320</c:v>
@@ -1139,19 +1139,19 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>319</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>296</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="370"/>
-          <c:min val="290"/>
+          <c:max val="390"/>
+          <c:min val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L85" sqref="L85"/>
+    <sheetView tabSelected="1" topLeftCell="D84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="1">
+        <v>45803</v>
+      </c>
+      <c r="D18">
+        <v>379</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45803</v>
+      </c>
+      <c r="G18">
+        <v>352</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">
@@ -4860,7 +4874,7 @@
         <v>45796</v>
       </c>
       <c r="D19">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="F19" s="1">
         <v>45796</v>

</xml_diff>

<commit_message>
LGHUB 2025/5/26 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD26D54-A292-430A-A769-AE1B6A8B4DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFDB774-19F6-4ED1-82C6-77A35DF6BDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>379</c:v>
+                  <c:v>385</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>379</c:v>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="390"/>
+          <c:max val="400"/>
           <c:min val="300"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="D83" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4860,7 +4860,7 @@
         <v>45803</v>
       </c>
       <c r="D18">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="F18" s="1">
         <v>45803</v>

</xml_diff>

<commit_message>
LGHUB 2025/5/30 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph.xlsx
+++ b/Documents/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFDB774-19F6-4ED1-82C6-77A35DF6BDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2869AB69-9D76-4A01-94DE-CEA62A6C9890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,10 +577,10 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>385</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>379</c:v>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>352</c:v>
+                  <c:v>354</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>349</c:v>
@@ -1797,10 +1797,10 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D83" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L85" sqref="L85"/>
+    <sheetView tabSelected="1" topLeftCell="D85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">
@@ -4860,13 +4860,13 @@
         <v>45803</v>
       </c>
       <c r="D18">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F18" s="1">
         <v>45803</v>
       </c>
       <c r="G18">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>